<commit_message>
All new updated cached data and processing scripts
Updated with new logic for parallel processing and using a common helper function for building the workplan species list. Changes in bispy package update data structures in the cached files.
</commit_message>
<xml_diff>
--- a/Data Release/sources/AdditionalSourceData.xlsx
+++ b/Data Release/sources/AdditionalSourceData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sbristol/github_usgs-bcb/FWS-ESA-WorkPlanSpecies/Data Release/sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB4FC9D-EDCB-B440-ADB8-D87BEFB483E0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43EBD074-B1BB-1046-BB79-55DE4DD07D3F}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8540" yWindow="2780" windowWidth="27640" windowHeight="16940" xr2:uid="{5D137541-72D1-D94F-9935-7B9A97C1F60C}"/>
+    <workbookView xWindow="1160" yWindow="980" windowWidth="27640" windowHeight="16940" xr2:uid="{5D137541-72D1-D94F-9935-7B9A97C1F60C}"/>
   </bookViews>
   <sheets>
     <sheet name="Extracted Species ECOS Links" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1157" uniqueCount="806">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1154" uniqueCount="807">
   <si>
     <t>Scientific Name</t>
   </si>
@@ -2593,6 +2593,9 @@
   </si>
   <si>
     <t>Aspidoscelis arizonae</t>
+  </si>
+  <si>
+    <t>Picoides arcticus</t>
   </si>
 </sst>
 </file>
@@ -3028,10 +3031,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3779960-B314-6046-9B60-35A5B769FF8F}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:C364"/>
+  <dimension ref="A1:C363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A344" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A337" workbookViewId="0">
+      <selection activeCell="B366" sqref="B366"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5418,7 +5421,7 @@
         <v>273</v>
       </c>
       <c r="B222" s="2" t="s">
-        <v>273</v>
+        <v>806</v>
       </c>
       <c r="C222" t="s">
         <v>403</v>
@@ -5426,1564 +5429,1553 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A223" s="2" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="B223" s="2" t="s">
-        <v>273</v>
+        <v>288</v>
       </c>
       <c r="C223" t="s">
-        <v>403</v>
+        <v>570</v>
       </c>
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A224" s="2" t="s">
-        <v>288</v>
+        <v>35</v>
       </c>
       <c r="B224" s="2" t="s">
-        <v>288</v>
+        <v>35</v>
       </c>
       <c r="C224" t="s">
-        <v>570</v>
+        <v>425</v>
       </c>
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A225" s="2" t="s">
-        <v>35</v>
+        <v>207</v>
       </c>
       <c r="B225" s="2" t="s">
-        <v>35</v>
+        <v>207</v>
       </c>
       <c r="C225" t="s">
-        <v>425</v>
+        <v>657</v>
       </c>
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A226" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="B226" s="2" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C226" t="s">
-        <v>657</v>
+        <v>640</v>
       </c>
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A227" s="2" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="B227" s="2" t="s">
-        <v>201</v>
+        <v>215</v>
       </c>
       <c r="C227" t="s">
-        <v>640</v>
+        <v>671</v>
       </c>
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A228" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="B228" s="2" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C228" t="s">
-        <v>671</v>
+        <v>387</v>
       </c>
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A229" s="2" t="s">
-        <v>217</v>
+        <v>120</v>
       </c>
       <c r="B229" s="2" t="s">
-        <v>217</v>
+        <v>120</v>
       </c>
       <c r="C229" t="s">
-        <v>387</v>
+        <v>426</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A230" s="2" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="B230" s="2" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C230" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A231" s="2" t="s">
-        <v>129</v>
+        <v>32</v>
       </c>
       <c r="B231" s="2" t="s">
-        <v>129</v>
+        <v>32</v>
       </c>
       <c r="C231" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A232" s="2" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="B232" s="2" t="s">
-        <v>32</v>
+        <v>124</v>
       </c>
       <c r="C232" t="s">
-        <v>428</v>
+        <v>429</v>
       </c>
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A233" s="2" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="B233" s="2" t="s">
-        <v>124</v>
+        <v>131</v>
       </c>
       <c r="C233" t="s">
-        <v>429</v>
+        <v>430</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A234" s="2" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>131</v>
+        <v>39</v>
       </c>
       <c r="C234" t="s">
-        <v>430</v>
+        <v>431</v>
       </c>
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A235" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B235" s="2" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="C235" t="s">
-        <v>431</v>
+        <v>413</v>
       </c>
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A236" s="2" t="s">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="B236" s="2" t="s">
-        <v>34</v>
+        <v>143</v>
       </c>
       <c r="C236" t="s">
-        <v>413</v>
+        <v>478</v>
       </c>
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A237" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="B237" s="2" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="C237" t="s">
-        <v>478</v>
+        <v>479</v>
       </c>
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A238" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="B238" s="2" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="C238" t="s">
-        <v>479</v>
+        <v>480</v>
       </c>
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A239" s="2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="B239" s="2" t="s">
-        <v>149</v>
+        <v>155</v>
       </c>
       <c r="C239" t="s">
-        <v>480</v>
+        <v>481</v>
       </c>
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A240" s="2" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="B240" s="2" t="s">
-        <v>155</v>
+        <v>136</v>
       </c>
       <c r="C240" t="s">
-        <v>481</v>
+        <v>482</v>
       </c>
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="2" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="B241" s="2" t="s">
-        <v>136</v>
+        <v>152</v>
       </c>
       <c r="C241" t="s">
-        <v>482</v>
+        <v>483</v>
       </c>
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="B242" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C242" t="s">
-        <v>483</v>
+        <v>484</v>
       </c>
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="B243" s="2" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C243" t="s">
-        <v>484</v>
+        <v>485</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B244" s="2" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C244" t="s">
-        <v>485</v>
+        <v>486</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="B245" s="2" t="s">
-        <v>134</v>
+        <v>142</v>
       </c>
       <c r="C245" t="s">
-        <v>486</v>
+        <v>487</v>
       </c>
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="2" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="B246" s="2" t="s">
-        <v>142</v>
+        <v>89</v>
       </c>
       <c r="C246" t="s">
-        <v>487</v>
+        <v>388</v>
       </c>
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="2" t="s">
-        <v>89</v>
+        <v>242</v>
       </c>
       <c r="B247" s="2" t="s">
-        <v>89</v>
+        <v>242</v>
       </c>
       <c r="C247" t="s">
-        <v>388</v>
+        <v>605</v>
       </c>
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="2" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="B248" s="2" t="s">
-        <v>242</v>
+        <v>254</v>
       </c>
       <c r="C248" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="C249" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="2" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="B250" s="2" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="C250" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>247</v>
+        <v>251</v>
       </c>
       <c r="C251" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="B252" s="2" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="C252" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B253" s="2" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C253" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="B254" s="2" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="C254" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="2" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="B255" s="2" t="s">
-        <v>246</v>
+        <v>261</v>
       </c>
       <c r="C255" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="2" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="B256" s="2" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="C256" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A257" s="2" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="B257" s="2" t="s">
-        <v>248</v>
+        <v>264</v>
       </c>
       <c r="C257" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A258" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B258" s="2" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="C258" t="s">
-        <v>615</v>
-      </c>
-    </row>
-    <row r="259" spans="1:3" x14ac:dyDescent="0.2">
+        <v>616</v>
+      </c>
+    </row>
+    <row r="259" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A259" s="2" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="B259" s="2" t="s">
-        <v>258</v>
+        <v>263</v>
       </c>
       <c r="C259" t="s">
-        <v>616</v>
-      </c>
-    </row>
-    <row r="260" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>617</v>
+      </c>
+    </row>
+    <row r="260" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A260" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B260" s="2" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C260" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A261" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B261" s="2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="C261" t="s">
-        <v>618</v>
+        <v>619</v>
       </c>
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A262" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="B262" s="2" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="C262" t="s">
-        <v>619</v>
+        <v>620</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A263" s="2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="B263" s="2" t="s">
-        <v>262</v>
+        <v>265</v>
       </c>
       <c r="C263" t="s">
-        <v>620</v>
+        <v>621</v>
       </c>
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A264" s="2" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B264" s="2" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="C264" t="s">
-        <v>621</v>
+        <v>622</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A265" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="B265" s="2" t="s">
-        <v>256</v>
-      </c>
-      <c r="C265" t="s">
-        <v>622</v>
+      <c r="A265" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="B265" s="3" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A266" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="B266" s="3" t="s">
-        <v>80</v>
+      <c r="A266" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="B266" s="2" t="s">
+        <v>268</v>
+      </c>
+      <c r="C266" t="s">
+        <v>658</v>
       </c>
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A267" s="2" t="s">
-        <v>268</v>
+        <v>114</v>
       </c>
       <c r="B267" s="2" t="s">
-        <v>268</v>
+        <v>114</v>
       </c>
       <c r="C267" t="s">
-        <v>658</v>
+        <v>404</v>
       </c>
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A268" s="2" t="s">
-        <v>114</v>
+        <v>300</v>
       </c>
       <c r="B268" s="2" t="s">
-        <v>114</v>
+        <v>300</v>
       </c>
       <c r="C268" t="s">
-        <v>404</v>
+        <v>432</v>
       </c>
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A269" s="2" t="s">
-        <v>300</v>
+        <v>347</v>
       </c>
       <c r="B269" s="2" t="s">
-        <v>300</v>
+        <v>347</v>
       </c>
       <c r="C269" t="s">
-        <v>432</v>
+        <v>672</v>
       </c>
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A270" s="2" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B270" s="2" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="C270" t="s">
-        <v>672</v>
+        <v>673</v>
       </c>
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A271" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="B271" s="2" t="s">
-        <v>338</v>
+        <v>348</v>
       </c>
       <c r="C271" t="s">
-        <v>673</v>
+        <v>674</v>
       </c>
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A272" s="2" t="s">
-        <v>348</v>
+        <v>214</v>
       </c>
       <c r="B272" s="2" t="s">
-        <v>348</v>
+        <v>214</v>
       </c>
       <c r="C272" t="s">
-        <v>674</v>
+        <v>675</v>
       </c>
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A273" s="2" t="s">
-        <v>214</v>
+        <v>331</v>
       </c>
       <c r="B273" s="2" t="s">
-        <v>214</v>
+        <v>331</v>
       </c>
       <c r="C273" t="s">
-        <v>675</v>
+        <v>676</v>
       </c>
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A274" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="B274" s="2" t="s">
-        <v>331</v>
+        <v>334</v>
       </c>
       <c r="C274" t="s">
-        <v>676</v>
+        <v>677</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A275" s="2" t="s">
-        <v>334</v>
+        <v>359</v>
       </c>
       <c r="B275" s="2" t="s">
-        <v>334</v>
+        <v>359</v>
       </c>
       <c r="C275" t="s">
-        <v>677</v>
+        <v>678</v>
       </c>
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A276" s="2" t="s">
-        <v>359</v>
+        <v>328</v>
       </c>
       <c r="B276" s="2" t="s">
-        <v>359</v>
+        <v>328</v>
       </c>
       <c r="C276" t="s">
-        <v>678</v>
+        <v>679</v>
       </c>
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A277" s="2" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="B277" s="2" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="C277" t="s">
-        <v>679</v>
+        <v>680</v>
       </c>
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A278" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="B278" s="2" t="s">
-        <v>337</v>
+        <v>333</v>
       </c>
       <c r="C278" t="s">
-        <v>680</v>
+        <v>681</v>
       </c>
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A279" s="2" t="s">
-        <v>333</v>
+        <v>299</v>
       </c>
       <c r="B279" s="2" t="s">
-        <v>333</v>
+        <v>299</v>
       </c>
       <c r="C279" t="s">
-        <v>681</v>
+        <v>433</v>
       </c>
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A280" s="2" t="s">
-        <v>299</v>
+        <v>342</v>
       </c>
       <c r="B280" s="2" t="s">
-        <v>299</v>
+        <v>342</v>
       </c>
       <c r="C280" t="s">
-        <v>433</v>
+        <v>682</v>
       </c>
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A281" s="2" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="B281" s="2" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C281" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A282" s="2" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="B282" s="2" t="s">
-        <v>336</v>
+        <v>344</v>
       </c>
       <c r="C282" t="s">
-        <v>683</v>
+        <v>434</v>
       </c>
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A283" s="2" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="B283" s="2" t="s">
-        <v>344</v>
+        <v>332</v>
       </c>
       <c r="C283" t="s">
-        <v>434</v>
+        <v>684</v>
       </c>
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A284" s="2" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="B284" s="2" t="s">
-        <v>332</v>
+        <v>341</v>
       </c>
       <c r="C284" t="s">
-        <v>684</v>
+        <v>685</v>
       </c>
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A285" s="2" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="B285" s="2" t="s">
-        <v>341</v>
+        <v>352</v>
       </c>
       <c r="C285" t="s">
-        <v>685</v>
+        <v>686</v>
       </c>
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A286" s="2" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="B286" s="2" t="s">
-        <v>352</v>
+        <v>335</v>
       </c>
       <c r="C286" t="s">
-        <v>686</v>
+        <v>687</v>
       </c>
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A287" s="2" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="B287" s="2" t="s">
-        <v>335</v>
+        <v>350</v>
       </c>
       <c r="C287" t="s">
-        <v>687</v>
+        <v>435</v>
       </c>
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A288" s="2" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="B288" s="2" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="C288" t="s">
-        <v>435</v>
-      </c>
-    </row>
-    <row r="289" spans="1:3" x14ac:dyDescent="0.2">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="289" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A289" s="2" t="s">
-        <v>361</v>
+        <v>216</v>
       </c>
       <c r="B289" s="2" t="s">
-        <v>361</v>
+        <v>803</v>
       </c>
       <c r="C289" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="290" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>437</v>
+      </c>
+    </row>
+    <row r="290" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A290" s="2" t="s">
-        <v>216</v>
+        <v>329</v>
       </c>
       <c r="B290" s="2" t="s">
-        <v>803</v>
+        <v>329</v>
       </c>
       <c r="C290" t="s">
-        <v>437</v>
+        <v>688</v>
       </c>
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A291" s="2" t="s">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="B291" s="2" t="s">
-        <v>329</v>
+        <v>345</v>
       </c>
       <c r="C291" t="s">
-        <v>688</v>
+        <v>438</v>
       </c>
     </row>
     <row r="292" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A292" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="B292" s="2" t="s">
-        <v>345</v>
+        <v>339</v>
       </c>
       <c r="C292" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A293" s="2" t="s">
-        <v>339</v>
-      </c>
-      <c r="B293" s="2" t="s">
-        <v>339</v>
+      <c r="A293" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="B293" s="7" t="s">
+        <v>362</v>
       </c>
       <c r="C293" t="s">
-        <v>439</v>
+        <v>689</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A294" s="7" t="s">
-        <v>362</v>
-      </c>
-      <c r="B294" s="7" t="s">
-        <v>362</v>
+      <c r="A294" s="2" t="s">
+        <v>301</v>
+      </c>
+      <c r="B294" s="2" t="s">
+        <v>301</v>
       </c>
       <c r="C294" t="s">
-        <v>689</v>
+        <v>440</v>
       </c>
     </row>
     <row r="295" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A295" s="2" t="s">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="B295" s="2" t="s">
-        <v>301</v>
+        <v>351</v>
       </c>
       <c r="C295" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="296" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A296" s="2" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="B296" s="2" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="C296" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
     </row>
     <row r="297" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A297" s="2" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
       <c r="B297" s="2" t="s">
-        <v>360</v>
+        <v>343</v>
       </c>
       <c r="C297" t="s">
-        <v>442</v>
+        <v>690</v>
       </c>
     </row>
     <row r="298" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A298" s="2" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="B298" s="2" t="s">
-        <v>343</v>
+        <v>357</v>
       </c>
       <c r="C298" t="s">
-        <v>690</v>
+        <v>443</v>
       </c>
     </row>
     <row r="299" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A299" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B299" s="2" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="C299" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
     </row>
     <row r="300" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A300" s="2" t="s">
-        <v>356</v>
+        <v>31</v>
       </c>
       <c r="B300" s="2" t="s">
-        <v>356</v>
+        <v>31</v>
       </c>
       <c r="C300" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
     </row>
     <row r="301" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A301" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="B301" s="2" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="C301" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
     </row>
     <row r="302" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A302" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B302" s="2" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C302" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
     </row>
     <row r="303" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A303" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="B303" s="2" t="s">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="C303" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A304" s="2" t="s">
-        <v>30</v>
+        <v>304</v>
       </c>
       <c r="B304" s="2" t="s">
-        <v>30</v>
+        <v>304</v>
       </c>
       <c r="C304" t="s">
-        <v>448</v>
+        <v>389</v>
       </c>
     </row>
     <row r="305" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A305" s="2" t="s">
-        <v>304</v>
+        <v>2</v>
       </c>
       <c r="B305" s="2" t="s">
-        <v>304</v>
+        <v>2</v>
       </c>
       <c r="C305" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A306" s="2" t="s">
-        <v>2</v>
+        <v>317</v>
       </c>
       <c r="B306" s="2" t="s">
-        <v>2</v>
+        <v>317</v>
       </c>
       <c r="C306" t="s">
-        <v>390</v>
+        <v>528</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A307" s="2" t="s">
-        <v>317</v>
+        <v>243</v>
       </c>
       <c r="B307" s="2" t="s">
-        <v>317</v>
+        <v>243</v>
       </c>
       <c r="C307" t="s">
-        <v>528</v>
+        <v>623</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A308" s="2" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="B308" s="2" t="s">
-        <v>243</v>
+        <v>322</v>
       </c>
       <c r="C308" t="s">
-        <v>623</v>
+        <v>624</v>
       </c>
     </row>
     <row r="309" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A309" s="2" t="s">
-        <v>322</v>
+        <v>1</v>
       </c>
       <c r="B309" s="2" t="s">
-        <v>322</v>
+        <v>1</v>
       </c>
       <c r="C309" t="s">
-        <v>624</v>
+        <v>391</v>
       </c>
     </row>
     <row r="310" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A310" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B310" s="2" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C310" t="s">
-        <v>391</v>
+        <v>392</v>
       </c>
     </row>
     <row r="311" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A311" s="2" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="B311" s="2" t="s">
-        <v>3</v>
+        <v>55</v>
       </c>
       <c r="C311" t="s">
-        <v>392</v>
+        <v>571</v>
       </c>
     </row>
     <row r="312" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A312" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B312" s="2" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C312" t="s">
-        <v>571</v>
+        <v>529</v>
       </c>
     </row>
     <row r="313" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A313" s="2" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="B313" s="2" t="s">
-        <v>52</v>
+        <v>98</v>
       </c>
       <c r="C313" t="s">
-        <v>529</v>
+        <v>572</v>
       </c>
     </row>
     <row r="314" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A314" s="2" t="s">
-        <v>98</v>
+        <v>194</v>
       </c>
       <c r="B314" s="2" t="s">
-        <v>98</v>
+        <v>194</v>
       </c>
       <c r="C314" t="s">
-        <v>572</v>
+        <v>573</v>
       </c>
     </row>
     <row r="315" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A315" s="2" t="s">
-        <v>194</v>
+        <v>91</v>
       </c>
       <c r="B315" s="2" t="s">
-        <v>194</v>
+        <v>91</v>
       </c>
       <c r="C315" t="s">
-        <v>573</v>
+        <v>449</v>
       </c>
     </row>
     <row r="316" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A316" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="B316" s="2" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="C316" t="s">
-        <v>449</v>
+        <v>659</v>
       </c>
     </row>
     <row r="317" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A317" s="2" t="s">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="B317" s="2" t="s">
-        <v>79</v>
+        <v>9</v>
       </c>
       <c r="C317" t="s">
-        <v>659</v>
+        <v>574</v>
       </c>
     </row>
     <row r="318" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A318" s="2" t="s">
-        <v>9</v>
+        <v>189</v>
       </c>
       <c r="B318" s="2" t="s">
-        <v>9</v>
+        <v>189</v>
       </c>
       <c r="C318" t="s">
-        <v>574</v>
+        <v>575</v>
       </c>
     </row>
     <row r="319" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A319" s="2" t="s">
-        <v>189</v>
+        <v>70</v>
       </c>
       <c r="B319" s="2" t="s">
-        <v>189</v>
+        <v>70</v>
       </c>
       <c r="C319" t="s">
-        <v>575</v>
+        <v>625</v>
       </c>
     </row>
     <row r="320" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A320" s="2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="B320" s="2" t="s">
-        <v>70</v>
+        <v>86</v>
       </c>
       <c r="C320" t="s">
-        <v>625</v>
+        <v>691</v>
       </c>
     </row>
     <row r="321" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A321" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="B321" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C321" t="s">
-        <v>691</v>
+        <v>692</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A322" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B322" s="2" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="C322" t="s">
-        <v>692</v>
+        <v>693</v>
       </c>
     </row>
     <row r="323" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A323" s="2" t="s">
-        <v>87</v>
+        <v>312</v>
       </c>
       <c r="B323" s="2" t="s">
-        <v>87</v>
+        <v>312</v>
       </c>
       <c r="C323" t="s">
-        <v>693</v>
+        <v>393</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A324" s="2" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="B324" s="2" t="s">
-        <v>312</v>
+        <v>293</v>
       </c>
       <c r="C324" t="s">
-        <v>393</v>
+        <v>626</v>
       </c>
     </row>
     <row r="325" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A325" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="B325" s="2" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C325" t="s">
-        <v>626</v>
+        <v>627</v>
       </c>
     </row>
     <row r="326" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A326" s="2" t="s">
-        <v>291</v>
+        <v>103</v>
       </c>
       <c r="B326" s="2" t="s">
-        <v>291</v>
+        <v>103</v>
       </c>
       <c r="C326" t="s">
-        <v>627</v>
+        <v>636</v>
       </c>
     </row>
     <row r="327" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A327" s="2" t="s">
-        <v>103</v>
+        <v>316</v>
       </c>
       <c r="B327" s="2" t="s">
-        <v>103</v>
+        <v>316</v>
       </c>
       <c r="C327" t="s">
-        <v>636</v>
+        <v>530</v>
       </c>
     </row>
     <row r="328" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A328" s="2" t="s">
-        <v>316</v>
+        <v>195</v>
       </c>
       <c r="B328" s="2" t="s">
-        <v>316</v>
+        <v>195</v>
       </c>
       <c r="C328" t="s">
-        <v>530</v>
-      </c>
-    </row>
-    <row r="329" spans="1:3" x14ac:dyDescent="0.2">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="329" spans="1:3" ht="32" x14ac:dyDescent="0.2">
       <c r="A329" s="2" t="s">
-        <v>195</v>
+        <v>211</v>
       </c>
       <c r="B329" s="2" t="s">
-        <v>195</v>
+        <v>801</v>
       </c>
       <c r="C329" t="s">
-        <v>576</v>
-      </c>
-    </row>
-    <row r="330" spans="1:3" ht="32" x14ac:dyDescent="0.2">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="330" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A330" s="2" t="s">
-        <v>211</v>
+        <v>56</v>
       </c>
       <c r="B330" s="2" t="s">
-        <v>801</v>
+        <v>56</v>
       </c>
       <c r="C330" t="s">
-        <v>660</v>
+        <v>577</v>
       </c>
     </row>
     <row r="331" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A331" s="2" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="B331" s="2" t="s">
-        <v>56</v>
+        <v>6</v>
       </c>
       <c r="C331" t="s">
-        <v>577</v>
+        <v>405</v>
       </c>
     </row>
     <row r="332" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A332" s="2" t="s">
-        <v>6</v>
+        <v>313</v>
       </c>
       <c r="B332" s="2" t="s">
-        <v>6</v>
+        <v>313</v>
       </c>
       <c r="C332" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A333" s="2" t="s">
-        <v>313</v>
+        <v>226</v>
       </c>
       <c r="B333" s="2" t="s">
-        <v>313</v>
+        <v>226</v>
       </c>
       <c r="C333" t="s">
-        <v>406</v>
+        <v>488</v>
       </c>
     </row>
     <row r="334" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A334" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="B334" s="2" t="s">
-        <v>226</v>
+        <v>232</v>
       </c>
       <c r="C334" t="s">
-        <v>488</v>
+        <v>489</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A335" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="B335" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C335" t="s">
-        <v>489</v>
+        <v>490</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A336" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B336" s="2" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C336" t="s">
-        <v>490</v>
+        <v>491</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A337" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="B337" s="2" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C337" t="s">
-        <v>491</v>
+        <v>492</v>
       </c>
     </row>
     <row r="338" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A338" s="2" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="B338" s="2" t="s">
-        <v>224</v>
+        <v>255</v>
       </c>
       <c r="C338" t="s">
-        <v>492</v>
+        <v>628</v>
       </c>
     </row>
     <row r="339" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A339" s="2" t="s">
-        <v>255</v>
+        <v>75</v>
       </c>
       <c r="B339" s="2" t="s">
-        <v>255</v>
+        <v>75</v>
       </c>
       <c r="C339" t="s">
-        <v>628</v>
+        <v>637</v>
       </c>
     </row>
     <row r="340" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A340" s="2" t="s">
-        <v>75</v>
+        <v>210</v>
       </c>
       <c r="B340" s="2" t="s">
-        <v>75</v>
+        <v>210</v>
       </c>
       <c r="C340" t="s">
-        <v>637</v>
+        <v>661</v>
       </c>
     </row>
     <row r="341" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A341" s="2" t="s">
-        <v>210</v>
+        <v>162</v>
       </c>
       <c r="B341" s="2" t="s">
-        <v>210</v>
+        <v>162</v>
       </c>
       <c r="C341" t="s">
-        <v>661</v>
+        <v>531</v>
       </c>
     </row>
     <row r="342" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A342" s="2" t="s">
-        <v>162</v>
+        <v>125</v>
       </c>
       <c r="B342" s="2" t="s">
-        <v>162</v>
+        <v>800</v>
       </c>
       <c r="C342" t="s">
-        <v>531</v>
+        <v>450</v>
       </c>
     </row>
     <row r="343" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A343" s="2" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B343" s="2" t="s">
-        <v>800</v>
+        <v>127</v>
       </c>
       <c r="C343" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
     </row>
     <row r="344" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A344" s="2" t="s">
-        <v>127</v>
+        <v>282</v>
       </c>
       <c r="B344" s="2" t="s">
-        <v>127</v>
+        <v>282</v>
       </c>
       <c r="C344" t="s">
-        <v>451</v>
+        <v>578</v>
       </c>
     </row>
     <row r="345" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A345" s="2" t="s">
-        <v>282</v>
+        <v>354</v>
       </c>
       <c r="B345" s="2" t="s">
-        <v>282</v>
+        <v>354</v>
       </c>
       <c r="C345" t="s">
-        <v>578</v>
+        <v>694</v>
       </c>
     </row>
     <row r="346" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A346" s="2" t="s">
-        <v>354</v>
+        <v>50</v>
       </c>
       <c r="B346" s="2" t="s">
-        <v>354</v>
+        <v>50</v>
       </c>
       <c r="C346" t="s">
-        <v>694</v>
+        <v>532</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A347" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B347" s="2" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="C347" t="s">
-        <v>532</v>
+        <v>452</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A348" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="B348" s="2" t="s">
-        <v>33</v>
+        <v>38</v>
       </c>
       <c r="C348" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
     </row>
     <row r="349" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A349" s="2" t="s">
-        <v>38</v>
+        <v>358</v>
       </c>
       <c r="B349" s="2" t="s">
-        <v>38</v>
+        <v>358</v>
       </c>
       <c r="C349" t="s">
-        <v>453</v>
+        <v>695</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A350" s="2" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="B350" s="2" t="s">
-        <v>358</v>
+        <v>340</v>
       </c>
       <c r="C350" t="s">
-        <v>695</v>
+        <v>696</v>
       </c>
     </row>
     <row r="351" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A351" s="2" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="B351" s="2" t="s">
-        <v>340</v>
+        <v>353</v>
       </c>
       <c r="C351" t="s">
-        <v>696</v>
+        <v>697</v>
       </c>
     </row>
     <row r="352" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A352" s="2" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="B352" s="2" t="s">
-        <v>353</v>
+        <v>346</v>
       </c>
       <c r="C352" t="s">
-        <v>697</v>
+        <v>698</v>
       </c>
     </row>
     <row r="353" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A353" s="2" t="s">
-        <v>346</v>
+        <v>85</v>
       </c>
       <c r="B353" s="2" t="s">
-        <v>346</v>
+        <v>85</v>
       </c>
       <c r="C353" t="s">
-        <v>698</v>
+        <v>699</v>
       </c>
     </row>
     <row r="354" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A354" s="2" t="s">
-        <v>85</v>
+        <v>327</v>
       </c>
       <c r="B354" s="2" t="s">
-        <v>85</v>
+        <v>327</v>
       </c>
       <c r="C354" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
     </row>
     <row r="355" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A355" s="2" t="s">
-        <v>327</v>
+        <v>28</v>
       </c>
       <c r="B355" s="2" t="s">
-        <v>327</v>
+        <v>28</v>
       </c>
       <c r="C355" t="s">
-        <v>700</v>
+        <v>407</v>
       </c>
     </row>
     <row r="356" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A356" s="2" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="B356" s="2" t="s">
-        <v>28</v>
+        <v>90</v>
       </c>
       <c r="C356" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
     </row>
     <row r="357" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A357" s="2" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="B357" s="2" t="s">
-        <v>90</v>
+        <v>793</v>
       </c>
       <c r="C357" t="s">
-        <v>408</v>
+        <v>701</v>
       </c>
     </row>
     <row r="358" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A358" s="2" t="s">
-        <v>20</v>
+        <v>330</v>
       </c>
       <c r="B358" s="2" t="s">
-        <v>793</v>
+        <v>330</v>
       </c>
       <c r="C358" t="s">
-        <v>701</v>
+        <v>702</v>
       </c>
     </row>
     <row r="359" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A359" s="2" t="s">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="B359" s="2" t="s">
-        <v>330</v>
+        <v>355</v>
       </c>
       <c r="C359" t="s">
-        <v>702</v>
+        <v>703</v>
       </c>
     </row>
     <row r="360" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A360" s="2" t="s">
-        <v>355</v>
+        <v>192</v>
       </c>
       <c r="B360" s="2" t="s">
-        <v>355</v>
+        <v>192</v>
       </c>
       <c r="C360" t="s">
-        <v>703</v>
+        <v>579</v>
       </c>
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A361" s="2" t="s">
-        <v>192</v>
+        <v>122</v>
       </c>
       <c r="B361" s="2" t="s">
-        <v>192</v>
+        <v>122</v>
       </c>
       <c r="C361" t="s">
-        <v>579</v>
+        <v>454</v>
       </c>
     </row>
     <row r="362" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A362" s="2" t="s">
-        <v>122</v>
+        <v>323</v>
       </c>
       <c r="B362" s="2" t="s">
-        <v>122</v>
+        <v>323</v>
       </c>
       <c r="C362" t="s">
-        <v>454</v>
+        <v>638</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A363" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="B363" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="C363" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="364" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A364" s="8" t="s">
+      <c r="A363" s="8" t="s">
         <v>318</v>
       </c>
-      <c r="B364" s="3" t="s">
+      <c r="B363" s="3" t="s">
         <v>318</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:C1" xr:uid="{7FED1E93-0448-5F4A-A3C7-7D41DB1E4D82}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C364">
-      <sortCondition ref="B1:B364"/>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:C363">
+      <sortCondition ref="B1:B363"/>
     </sortState>
   </autoFilter>
   <hyperlinks>
@@ -7011,13 +7003,13 @@
     <hyperlink ref="A154" r:id="rId22" display="https://ecos.fws.gov/ecp/species/6607" xr:uid="{1426E751-3F20-2148-88F3-BFFEDE8D2721}"/>
     <hyperlink ref="A186" r:id="rId23" display="https://ecos.fws.gov/ecp/species/6772" xr:uid="{B48C4C34-4C05-BA4B-A49E-AAAEA1F5856C}"/>
     <hyperlink ref="A187" r:id="rId24" display="https://ecos.fws.gov/ecp/species/5856" xr:uid="{C74788F0-B62A-CC47-AAE8-FA710D22D80A}"/>
-    <hyperlink ref="A229" r:id="rId25" display="https://ecos.fws.gov/ecp/species/3529" xr:uid="{ED7DF352-7F4C-0A47-A60E-86FE701090F7}"/>
-    <hyperlink ref="A247" r:id="rId26" display="https://ecos.fws.gov/ecp/species/455" xr:uid="{90F9863B-E104-3746-8BCD-F2AC0D292ECA}"/>
-    <hyperlink ref="A305" r:id="rId27" display="https://ecos.fws.gov/ecp/species/5133" xr:uid="{12E160DA-5707-7041-90F3-30571EA6AD3E}"/>
-    <hyperlink ref="A306" r:id="rId28" display="https://ecos.fws.gov/ecp/species/7827" xr:uid="{3A026900-0BED-244C-AD71-BC311843105A}"/>
-    <hyperlink ref="A310" r:id="rId29" display="https://ecos.fws.gov/ecp/species/1375" xr:uid="{150EED52-BAF7-A541-95E7-6867DE2456CD}"/>
-    <hyperlink ref="A311" r:id="rId30" display="https://ecos.fws.gov/ecp/species/3376" xr:uid="{58E3F09E-4B6D-6149-88BD-7B6D261EF31F}"/>
-    <hyperlink ref="A324" r:id="rId31" display="https://ecos.fws.gov/ecp/species/5425" xr:uid="{5BF188E6-BEAE-0B47-AD99-A8AA80D56DC3}"/>
+    <hyperlink ref="A228" r:id="rId25" display="https://ecos.fws.gov/ecp/species/3529" xr:uid="{ED7DF352-7F4C-0A47-A60E-86FE701090F7}"/>
+    <hyperlink ref="A246" r:id="rId26" display="https://ecos.fws.gov/ecp/species/455" xr:uid="{90F9863B-E104-3746-8BCD-F2AC0D292ECA}"/>
+    <hyperlink ref="A304" r:id="rId27" display="https://ecos.fws.gov/ecp/species/5133" xr:uid="{12E160DA-5707-7041-90F3-30571EA6AD3E}"/>
+    <hyperlink ref="A305" r:id="rId28" display="https://ecos.fws.gov/ecp/species/7827" xr:uid="{3A026900-0BED-244C-AD71-BC311843105A}"/>
+    <hyperlink ref="A309" r:id="rId29" display="https://ecos.fws.gov/ecp/species/1375" xr:uid="{150EED52-BAF7-A541-95E7-6867DE2456CD}"/>
+    <hyperlink ref="A310" r:id="rId30" display="https://ecos.fws.gov/ecp/species/3376" xr:uid="{58E3F09E-4B6D-6149-88BD-7B6D261EF31F}"/>
+    <hyperlink ref="A323" r:id="rId31" display="https://ecos.fws.gov/ecp/species/5425" xr:uid="{5BF188E6-BEAE-0B47-AD99-A8AA80D56DC3}"/>
     <hyperlink ref="A6" r:id="rId32" display="https://ecos.fws.gov/ecp/species/3910" xr:uid="{7B80E261-5BF9-6942-A338-016FBA71146B}"/>
     <hyperlink ref="A11" r:id="rId33" display="https://ecos.fws.gov/ecp/species/9022" xr:uid="{EA9245F9-8CDE-0D48-91C7-6CF485579E20}"/>
     <hyperlink ref="A15" r:id="rId34" display="https://ecos.fws.gov/ecp/species/9775" xr:uid="{706F4104-1A4F-6D45-B5F1-8CE9FC688CA3}"/>
@@ -7028,307 +7020,306 @@
     <hyperlink ref="A160" r:id="rId39" display="https://ecos.fws.gov/ecp/species/9234" xr:uid="{DE8A26D6-0745-034B-9829-DC1380318E33}"/>
     <hyperlink ref="A165" r:id="rId40" display="https://ecos.fws.gov/ecp/species/7717" xr:uid="{15755369-E6D3-4045-A37E-BC2879BFFAA2}"/>
     <hyperlink ref="A222" r:id="rId41" display="https://ecos.fws.gov/ecp/species/7951" xr:uid="{29F84CB5-7520-1B40-8B7D-698671B08EAF}"/>
-    <hyperlink ref="A223" r:id="rId42" display="https://ecos.fws.gov/ecp/species/7951" xr:uid="{78C67BC4-742A-DE42-8546-82CE4942CE49}"/>
-    <hyperlink ref="A268" r:id="rId43" display="https://ecos.fws.gov/ecp/species/4748" xr:uid="{D6A80F96-E67C-9248-8B93-DB514A0AA157}"/>
-    <hyperlink ref="A332" r:id="rId44" display="https://ecos.fws.gov/ecp/species/1123" xr:uid="{2327E9D8-03CC-D444-B3D9-9A258367AFA5}"/>
-    <hyperlink ref="A333" r:id="rId45" display="https://ecos.fws.gov/ecp/species/7266" xr:uid="{58F3BDC2-A1C9-C043-8806-EE9B241A1797}"/>
-    <hyperlink ref="A356" r:id="rId46" display="https://ecos.fws.gov/ecp/species/1924" xr:uid="{E9C68340-A8B5-6D4B-B843-B2CC10A96B1A}"/>
-    <hyperlink ref="A357" r:id="rId47" display="https://ecos.fws.gov/ecp/species/8745" xr:uid="{BAA30E52-B6D7-9942-9537-6242538ACB3C}"/>
-    <hyperlink ref="A7" r:id="rId48" display="https://ecos.fws.gov/ecp/species/9871" xr:uid="{3CAF6253-BEDA-2B4E-AB77-3CB3F288456E}"/>
-    <hyperlink ref="A8" r:id="rId49" display="https://ecos.fws.gov/ecp/species/785" xr:uid="{9B415958-C9C0-7E47-9ED4-69DCEA8ED60B}"/>
-    <hyperlink ref="A18" r:id="rId50" display="https://ecos.fws.gov/ecp/species/9873" xr:uid="{8A41C26E-EB2E-6D46-9037-07B8CDA71829}"/>
-    <hyperlink ref="A80" r:id="rId51" display="https://ecos.fws.gov/ecp/species/6895" xr:uid="{5D628A9F-F97A-6D4F-80C8-0E2B6A3E0966}"/>
-    <hyperlink ref="A236" r:id="rId52" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=F04A" xr:uid="{0C77E00D-7479-2546-92D1-E8848E5AA481}"/>
-    <hyperlink ref="A91" r:id="rId53" display="https://ecos.fws.gov/ecp/species/4511" xr:uid="{4E13999E-400D-3747-889F-EA2EB7DD1966}"/>
-    <hyperlink ref="A126" r:id="rId54" display="https://ecos.fws.gov/ecp/species/10339" xr:uid="{233FCAF0-5E24-4D4D-B962-A75DE9ECE53E}"/>
-    <hyperlink ref="A127" r:id="rId55" display="https://ecos.fws.gov/ecp/species/5164" xr:uid="{851A08BA-1420-F04F-A6DA-04EB37A7885C}"/>
-    <hyperlink ref="A128" r:id="rId56" display="https://ecos.fws.gov/ecp/species/9880" xr:uid="{35FB8694-887A-3B43-BC8D-B66E2DD9D878}"/>
-    <hyperlink ref="A161" r:id="rId57" display="https://ecos.fws.gov/ecp/species/9041" xr:uid="{7B59DEF7-F228-8C4F-AAD2-5882E9C1D5B0}"/>
-    <hyperlink ref="A162" r:id="rId58" display="https://ecos.fws.gov/ecp/species/7540" xr:uid="{7E64CC29-B338-C941-A539-6A27E0EDB847}"/>
-    <hyperlink ref="A163" r:id="rId59" display="https://ecos.fws.gov/ecp/species/783" xr:uid="{892C26C0-0086-CA45-8C07-EF4D32F6D475}"/>
-    <hyperlink ref="A164" r:id="rId60" display="https://ecos.fws.gov/ecp/species/7541" xr:uid="{0E357956-E3E5-9F45-9EBD-4D987C457F75}"/>
-    <hyperlink ref="A180" r:id="rId61" display="https://ecos.fws.gov/ecp/species/9881" xr:uid="{C79F7F02-2064-F34B-A701-ACFB26818322}"/>
-    <hyperlink ref="A197" r:id="rId62" display="https://ecos.fws.gov/ecp/species/9879" xr:uid="{61D6C1A0-2EB2-4942-A04D-4549011B7484}"/>
-    <hyperlink ref="A198" r:id="rId63" display="https://ecos.fws.gov/ecp/species/9883" xr:uid="{8D019D16-00BB-4445-8133-0215EF2A30BA}"/>
-    <hyperlink ref="A225" r:id="rId64" display="https://ecos.fws.gov/ecp/species/3533" xr:uid="{8D550F40-E620-FC4F-A68E-D94B4A821B3F}"/>
-    <hyperlink ref="A230" r:id="rId65" display="https://ecos.fws.gov/ecp/species/4693" xr:uid="{1D58E5BA-28A6-6F4D-B838-6498056FEBA7}"/>
-    <hyperlink ref="A231" r:id="rId66" display="https://ecos.fws.gov/ecp/species/3254" xr:uid="{02AAC49B-8BCC-4A4E-A34E-2102F63D1E29}"/>
-    <hyperlink ref="A232" r:id="rId67" display="https://ecos.fws.gov/ecp/species/10233" xr:uid="{FEADB3DB-0ED3-EA4A-8E3C-0A67707938AE}"/>
-    <hyperlink ref="A233" r:id="rId68" display="https://ecos.fws.gov/ecp/species/1937" xr:uid="{CDEC4061-FB93-F349-BBFE-7D736A2A8647}"/>
-    <hyperlink ref="A234" r:id="rId69" display="https://ecos.fws.gov/ecp/species/9887" xr:uid="{6D223629-DED1-9F44-A73D-2FAC5194E064}"/>
-    <hyperlink ref="A235" r:id="rId70" display="https://ecos.fws.gov/ecp/species/299" xr:uid="{F0074253-8EC8-BF46-AEEE-9CAA1371D397}"/>
-    <hyperlink ref="A269" r:id="rId71" display="https://ecos.fws.gov/ecp/species/8977" xr:uid="{BCB508DA-C3AC-F045-88C6-69AD75702B22}"/>
-    <hyperlink ref="A280" r:id="rId72" display="https://ecos.fws.gov/ecp/species/8984" xr:uid="{44F4B2A7-A544-264C-A1D2-BF046FF89B49}"/>
-    <hyperlink ref="A283" r:id="rId73" display="https://ecos.fws.gov/ecp/species/8986" xr:uid="{C834ECBB-37B9-1B42-86E5-9E3AAA949919}"/>
-    <hyperlink ref="A288" r:id="rId74" display="https://ecos.fws.gov/ecp/species/8991" xr:uid="{6B479769-5436-4B49-9A34-840C18BF88E6}"/>
-    <hyperlink ref="A289" r:id="rId75" display="https://ecos.fws.gov/ecp/species/8992" xr:uid="{E423C902-DC5D-E24E-BB1F-D7975BEAB797}"/>
-    <hyperlink ref="A290" r:id="rId76" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?sId=3974" xr:uid="{20E8A83E-8158-6B49-8D04-718FB5F66D83}"/>
-    <hyperlink ref="A292" r:id="rId77" display="https://ecos.fws.gov/ecp/species/2997" xr:uid="{5A1E9E5C-870C-EA49-80DF-8EC460C723C9}"/>
-    <hyperlink ref="A293" r:id="rId78" display="https://ecos.fws.gov/ecp/species/8995" xr:uid="{A117B146-3A81-D643-A5CD-47F117C9E584}"/>
-    <hyperlink ref="A295" r:id="rId79" display="https://ecos.fws.gov/ecp/species/8997" xr:uid="{11EF2442-A73B-6D4F-9FCA-2028DD48665C}"/>
-    <hyperlink ref="A296" r:id="rId80" display="https://ecos.fws.gov/ecp/species/8998" xr:uid="{1DF8CDE8-D5C5-6A4F-B635-25F3A3CA3AFC}"/>
-    <hyperlink ref="A297" r:id="rId81" display="https://ecos.fws.gov/ecp/species/8999" xr:uid="{DCD88F6A-67A1-6940-88D5-7CF452565E6B}"/>
-    <hyperlink ref="A299" r:id="rId82" display="https://ecos.fws.gov/ecp/species/9001" xr:uid="{9619CEDF-A496-A744-BF6A-AB1AC2BC9C63}"/>
-    <hyperlink ref="A300" r:id="rId83" display="https://ecos.fws.gov/ecp/species/9002" xr:uid="{36AE747F-A627-824A-9EB7-270C43E7661F}"/>
-    <hyperlink ref="A301" r:id="rId84" display="https://ecos.fws.gov/ecp/species/9042" xr:uid="{57C32620-21EF-4C4F-9D4A-B61AA95A8150}"/>
-    <hyperlink ref="A302" r:id="rId85" display="https://ecos.fws.gov/ecp/species/8967" xr:uid="{30D23C50-B8E2-7A45-BC14-26D58A4B9D17}"/>
-    <hyperlink ref="A303" r:id="rId86" display="https://ecos.fws.gov/ecp/species/8966" xr:uid="{A306EBCB-E2CE-E447-A8E1-97222AAD78E4}"/>
-    <hyperlink ref="A304" r:id="rId87" display="https://ecos.fws.gov/ecp/species/3963" xr:uid="{74BE6B4B-76AF-2E40-A138-2CC222EB1AC5}"/>
-    <hyperlink ref="A316" r:id="rId88" display="https://ecos.fws.gov/ecp/species/6208" xr:uid="{EED70E5B-9D26-2D49-90CA-118870A6E0FA}"/>
-    <hyperlink ref="A343" r:id="rId89" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?sId=8210" xr:uid="{DFED493E-EB40-5F46-AA73-A2E984E07853}"/>
-    <hyperlink ref="A344" r:id="rId90" display="https://ecos.fws.gov/ecp/species/7155" xr:uid="{1E34E677-E7C4-F249-A90C-2402FC5F8A34}"/>
-    <hyperlink ref="A348" r:id="rId91" display="https://ecos.fws.gov/ecp/species/7870" xr:uid="{93FABF54-3545-A24E-B617-EF15784A392A}"/>
-    <hyperlink ref="A349" r:id="rId92" display="https://ecos.fws.gov/ecp/species/8965" xr:uid="{0B5D3D0F-B248-D14F-A29E-7636E0459AF9}"/>
-    <hyperlink ref="A362" r:id="rId93" display="https://ecos.fws.gov/ecp/species/8209" xr:uid="{13123EB5-DF8F-0F42-A39E-E7A8A5B75CDB}"/>
-    <hyperlink ref="A46" r:id="rId94" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?sId=9860" xr:uid="{7C275CBF-8704-8E44-B8BA-4CEE7B08D9ED}"/>
-    <hyperlink ref="A49" r:id="rId95" display="https://ecos.fws.gov/ecp/species/9790" xr:uid="{72F112BE-6B1C-9742-B355-0718779B0AE5}"/>
-    <hyperlink ref="A50" r:id="rId96" display="https://ecos.fws.gov/ecp/species/9791" xr:uid="{451F3A23-F47B-1947-A485-1DC07C1E25E7}"/>
-    <hyperlink ref="A51" r:id="rId97" display="https://ecos.fws.gov/ecp/species/9792" xr:uid="{667508AB-7DA5-0F42-84A5-E7E671BDF9E1}"/>
-    <hyperlink ref="A52" r:id="rId98" display="https://ecos.fws.gov/ecp/species/9795" xr:uid="{9FC691A8-AF83-3645-B286-2447CDDC976A}"/>
-    <hyperlink ref="A53" r:id="rId99" display="https://ecos.fws.gov/ecp/species/4851" xr:uid="{7D9121C3-B9DD-8344-A871-9F8A31F2C592}"/>
-    <hyperlink ref="A54" r:id="rId100" display="https://ecos.fws.gov/ecp/species/9798" xr:uid="{28F1E893-3EE0-8D48-9848-69FAE8B37850}"/>
-    <hyperlink ref="A55" r:id="rId101" display="https://ecos.fws.gov/ecp/species/8539" xr:uid="{31A57676-4633-DA49-9DE6-C9D888CA1AA9}"/>
-    <hyperlink ref="A56" r:id="rId102" display="https://ecos.fws.gov/ecp/species/2605" xr:uid="{E5C360BB-492B-0D40-AFD6-07244CED5CF0}"/>
-    <hyperlink ref="A57" r:id="rId103" display="https://ecos.fws.gov/ecp/species/9801" xr:uid="{26D1E814-4F2E-4A40-8FA5-5EE500D86A2B}"/>
-    <hyperlink ref="A58" r:id="rId104" display="https://ecos.fws.gov/ecp/species/9803" xr:uid="{49020F91-2F3B-1B44-8495-FDDB64DD5320}"/>
-    <hyperlink ref="A61" r:id="rId105" display="https://ecos.fws.gov/ecp/species/9806" xr:uid="{7D04C721-CDFE-8943-80F0-247E98032568}"/>
-    <hyperlink ref="A121" r:id="rId106" display="https://ecos.fws.gov/ecp/species/5458" xr:uid="{D9C09780-CC8A-3C46-B019-49E73CEC5353}"/>
-    <hyperlink ref="A122" r:id="rId107" display="https://ecos.fws.gov/ecp/species/3289" xr:uid="{BCCE5561-28DB-BE4B-A2AB-DB1F9BAEE17F}"/>
-    <hyperlink ref="A149" r:id="rId108" display="https://ecos.fws.gov/ecp/species/9812" xr:uid="{6AB9325A-47DD-3941-9C6B-423985C60546}"/>
-    <hyperlink ref="A150" r:id="rId109" display="https://ecos.fws.gov/ecp/species/9813" xr:uid="{FB5C6046-E333-CF46-B1BF-6DFAD09111E6}"/>
-    <hyperlink ref="A151" r:id="rId110" display="https://ecos.fws.gov/ecp/species/9821" xr:uid="{8DB52BEB-8CD8-EC4B-9FA0-9BFE61257268}"/>
-    <hyperlink ref="A172" r:id="rId111" display="https://ecos.fws.gov/ecp/species/2692" xr:uid="{AB12A771-75D0-4848-AD27-F9A5AD5E3378}"/>
-    <hyperlink ref="A202" r:id="rId112" display="https://ecos.fws.gov/ecp/species/9815" xr:uid="{6984288D-6B1B-894D-A154-02CFF6FA93B9}"/>
-    <hyperlink ref="A203" r:id="rId113" display="https://ecos.fws.gov/ecp/species/9816" xr:uid="{AF88B8E7-4B6D-034A-9430-EBD6C1800EDF}"/>
-    <hyperlink ref="A204" r:id="rId114" display="https://ecos.fws.gov/ecp/species/9823" xr:uid="{4DFF5E55-762E-E844-BE02-9383D709EFBF}"/>
-    <hyperlink ref="A207" r:id="rId115" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=K07Q" xr:uid="{90CCD8F2-03C3-B741-AF81-F1AF45C9FC57}"/>
-    <hyperlink ref="A208" r:id="rId116" display="https://ecos.fws.gov/ecp/species/8226" xr:uid="{0EFD34B4-77C5-AA49-9CC3-4BB3D613D63E}"/>
-    <hyperlink ref="A237" r:id="rId117" display="https://ecos.fws.gov/ecp/species/6542" xr:uid="{DADE2C4D-0227-984F-8F70-BD2D0C8B169C}"/>
-    <hyperlink ref="A238" r:id="rId118" display="https://ecos.fws.gov/ecp/species/3812" xr:uid="{FB209C52-F21A-AF44-B559-18D122CB78CD}"/>
-    <hyperlink ref="A239" r:id="rId119" display="https://ecos.fws.gov/ecp/species/8915" xr:uid="{6F877B72-DF29-1A41-B332-3074BCDFC9C8}"/>
-    <hyperlink ref="A240" r:id="rId120" display="https://ecos.fws.gov/ecp/species/4532" xr:uid="{E1987221-660D-1644-B48C-5F791F1C3C2E}"/>
-    <hyperlink ref="A241" r:id="rId121" display="https://ecos.fws.gov/ecp/species/9827" xr:uid="{2D51B487-5D39-0843-A37E-FA40ADD408D6}"/>
-    <hyperlink ref="A242" r:id="rId122" display="https://ecos.fws.gov/ecp/species/5071" xr:uid="{F7C139B6-F278-C44D-848D-63F91B5C85C6}"/>
-    <hyperlink ref="A243" r:id="rId123" display="https://ecos.fws.gov/ecp/species/9832" xr:uid="{E2277873-671A-1845-809D-3BC28AC6C186}"/>
-    <hyperlink ref="A244" r:id="rId124" display="https://ecos.fws.gov/ecp/species/6252" xr:uid="{75ADEA4D-4E00-EF4A-9E26-8022DC586754}"/>
-    <hyperlink ref="A245" r:id="rId125" display="https://ecos.fws.gov/ecp/species/6815" xr:uid="{4AFC468D-A9FE-BB4D-9851-9BB54453E642}"/>
-    <hyperlink ref="A246" r:id="rId126" display="https://ecos.fws.gov/ecp/species/9837" xr:uid="{4AF342DA-11D9-AC49-9B84-50CEC76DFA53}"/>
-    <hyperlink ref="A334" r:id="rId127" display="https://ecos.fws.gov/ecp/species/5908" xr:uid="{A66DDBD4-E9EF-E344-8EF4-AA102BC5CE50}"/>
-    <hyperlink ref="A335" r:id="rId128" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=K007" xr:uid="{154407DE-4A70-FD48-95B6-5F264B73D503}"/>
-    <hyperlink ref="A336" r:id="rId129" display="https://ecos.fws.gov/ecp/species/3150" xr:uid="{12B65F36-DF9E-F94C-B891-007649A291E7}"/>
-    <hyperlink ref="A337" r:id="rId130" display="https://ecos.fws.gov/ecp/species/7901" xr:uid="{BA3DE6B8-A1DF-5E42-92E0-9F7345A48D75}"/>
-    <hyperlink ref="A338" r:id="rId131" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=K04R" xr:uid="{919A27E2-9F84-8B42-80E1-A566D0ADA50D}"/>
-    <hyperlink ref="A12" r:id="rId132" display="https://ecos.fws.gov/ecp/species/3966" xr:uid="{6A4C802F-39BC-C043-AFBF-47D182426F3D}"/>
-    <hyperlink ref="A65" r:id="rId133" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=E0AR" xr:uid="{B94DF11E-3BB4-EE4D-AC8E-1EFEB90B39B8}"/>
-    <hyperlink ref="A73" r:id="rId134" display="https://ecos.fws.gov/ecp/species/5634" xr:uid="{2FEE5F92-AD02-B044-92AD-59BF79229CA6}"/>
-    <hyperlink ref="A78" r:id="rId135" display="https://ecos.fws.gov/ecp/species/5162" xr:uid="{5BA51E07-DF2C-E843-BB27-39EA050713BE}"/>
-    <hyperlink ref="A79" r:id="rId136" display="https://ecos.fws.gov/ecp/species/5883" xr:uid="{0BBC2D63-CDA5-4746-9D42-EEC73B64A316}"/>
-    <hyperlink ref="A88" r:id="rId137" display="https://ecos.fws.gov/ecp/species/5605" xr:uid="{4367DD89-7045-5A4C-AA50-910A6F89BF12}"/>
-    <hyperlink ref="A96" r:id="rId138" display="https://ecos.fws.gov/ecp/species/9851" xr:uid="{04157E71-1250-8C4C-8569-D3E20F37EFFF}"/>
-    <hyperlink ref="A99" r:id="rId139" display="https://ecos.fws.gov/ecp/species/5601" xr:uid="{19B03DAE-CDDD-3242-80DE-40A817488237}"/>
-    <hyperlink ref="A100" r:id="rId140" display="https://ecos.fws.gov/ecp/species/3117" xr:uid="{D9B8D077-FE01-6F41-AEDA-0A7DCB1D1C02}"/>
-    <hyperlink ref="A101" r:id="rId141" display="https://ecos.fws.gov/ecp/species/4984" xr:uid="{97D9F208-52A1-A248-83BC-B4C7049505B2}"/>
-    <hyperlink ref="A103" r:id="rId142" display="https://ecos.fws.gov/ecp/species/9852" xr:uid="{41A119D1-1FCF-AD4E-9980-710F9917976F}"/>
-    <hyperlink ref="A104" r:id="rId143" display="https://ecos.fws.gov/ecp/species/1396" xr:uid="{F5035606-4266-8148-8759-8A95CDC8847E}"/>
-    <hyperlink ref="A105" r:id="rId144" display="https://ecos.fws.gov/ecp/species/300" xr:uid="{55D943C2-8BFC-8246-8893-82EC311A6A8E}"/>
-    <hyperlink ref="A106" r:id="rId145" display="https://ecos.fws.gov/ecp/species/9854" xr:uid="{7F0F2FE9-E9BA-DE4B-A68E-265EB2FD7919}"/>
-    <hyperlink ref="A107" r:id="rId146" display="https://ecos.fws.gov/ecp/species/8219" xr:uid="{CF79CE6E-FEFF-D64D-AD3C-4C5B4B1641D7}"/>
-    <hyperlink ref="A124" r:id="rId147" display="https://ecos.fws.gov/ecp/species/9171" xr:uid="{A6B499D7-22C0-A140-BFF9-0167DB934640}"/>
-    <hyperlink ref="A125" r:id="rId148" display="https://ecos.fws.gov/ecp/species/5045" xr:uid="{9F3E29E7-3F1C-2D44-BBA0-B415A9F35381}"/>
-    <hyperlink ref="A129" r:id="rId149" display="https://ecos.fws.gov/ecp/species/627" xr:uid="{05BB08E2-B70B-984A-9ABA-BB9AB2506A0D}"/>
-    <hyperlink ref="A157" r:id="rId150" display="https://ecos.fws.gov/ecp/species/8217" xr:uid="{42376615-CFC2-B94F-BD90-CB313B2D1484}"/>
-    <hyperlink ref="A166" r:id="rId151" display="https://ecos.fws.gov/ecp/species/9298" xr:uid="{8E89C400-051D-754D-AD85-B8B1FCB944EC}"/>
-    <hyperlink ref="A168" r:id="rId152" display="https://ecos.fws.gov/ecp/species/6899" xr:uid="{3CD8C228-179F-9542-8F92-ACDCC2E59EB7}"/>
-    <hyperlink ref="A188" r:id="rId153" display="https://ecos.fws.gov/ecp/species/9855" xr:uid="{560CB0AA-5D97-7F44-B5C8-9C3F5EA610AD}"/>
-    <hyperlink ref="A189" r:id="rId154" display="https://ecos.fws.gov/ecp/species/3931" xr:uid="{2293F100-7AA3-5C47-9F93-7A17CCD29160}"/>
-    <hyperlink ref="A190" r:id="rId155" display="https://ecos.fws.gov/ecp/species/2994" xr:uid="{C5671D86-B2E5-B344-8F39-1E5B5ABF921F}"/>
-    <hyperlink ref="A191" r:id="rId156" display="https://ecos.fws.gov/ecp/species/528" xr:uid="{C0C0588C-4EA7-3B4B-86E5-C88838FCC5A7}"/>
-    <hyperlink ref="A192" r:id="rId157" display="https://ecos.fws.gov/ecp/species/3120" xr:uid="{FF835422-50C8-1840-A5B0-D081B0D9E598}"/>
-    <hyperlink ref="A193" r:id="rId158" display="https://ecos.fws.gov/ecp/species/9861" xr:uid="{A6ECB29D-F146-C34C-BA9B-EC9AA79A5EAF}"/>
-    <hyperlink ref="A194" r:id="rId159" display="https://ecos.fws.gov/ecp/species/2800" xr:uid="{1AF230A5-D505-A44F-B357-B894599D81AF}"/>
-    <hyperlink ref="A195" r:id="rId160" display="https://ecos.fws.gov/ecp/species/2576" xr:uid="{613C4046-2DF5-5244-88F4-0F47A736B92F}"/>
-    <hyperlink ref="A214" r:id="rId161" display="https://ecos.fws.gov/ecp/species/9863" xr:uid="{7B1C05F6-BE4C-1443-A55D-D32DA5532DD0}"/>
-    <hyperlink ref="A215" r:id="rId162" display="https://ecos.fws.gov/ecp/species/6211" xr:uid="{E325B52F-5C96-F34C-9476-35EB20E37748}"/>
-    <hyperlink ref="A216" r:id="rId163" display="https://ecos.fws.gov/ecp/species/9864" xr:uid="{9CD96110-BC8C-924E-B6D3-EF8CA0A61FAD}"/>
-    <hyperlink ref="A217" r:id="rId164" display="https://ecos.fws.gov/ecp/species/5431" xr:uid="{16D4A496-E1C7-7141-BDD7-276F725021B3}"/>
-    <hyperlink ref="A218" r:id="rId165" display="https://ecos.fws.gov/ecp/species/1773" xr:uid="{2CB73C16-3985-FC43-AAFD-9FAEE4DF5FAB}"/>
-    <hyperlink ref="A219" r:id="rId166" display="https://ecos.fws.gov/ecp/species/9866" xr:uid="{F914A8AF-884A-4C4E-B108-CCFEA654F885}"/>
-    <hyperlink ref="A307" r:id="rId167" display="https://ecos.fws.gov/ecp/species/3416" xr:uid="{08F039F4-252C-634C-BAF4-2B3456409F68}"/>
-    <hyperlink ref="A313" r:id="rId168" display="https://ecos.fws.gov/ecp/species/7544" xr:uid="{99EE4CF0-37B7-B747-A65B-B1FE615ABC3C}"/>
-    <hyperlink ref="A328" r:id="rId169" display="https://ecos.fws.gov/ecp/species/9011" xr:uid="{FCD9C05F-292A-1B4B-AD9E-522E77F8F511}"/>
-    <hyperlink ref="A342" r:id="rId170" display="https://ecos.fws.gov/ecp/species/9868" xr:uid="{F92A75AD-F5B8-4E42-9C87-4EFCB7AC248A}"/>
-    <hyperlink ref="A347" r:id="rId171" display="https://ecos.fws.gov/ecp/species/4398" xr:uid="{688A5CC8-471D-8D4F-B2C7-A5F48CE80690}"/>
-    <hyperlink ref="A4" r:id="rId172" display="https://ecos.fws.gov/ecp/species/9918" xr:uid="{724C8741-2014-0447-B126-860B34D0CD4A}"/>
-    <hyperlink ref="A10" r:id="rId173" display="https://ecos.fws.gov/ecp/species/2364" xr:uid="{B3955CAA-1DC9-7345-B8BB-F60AA23DE765}"/>
-    <hyperlink ref="A16" r:id="rId174" display="https://ecos.fws.gov/ecp/species/5310" xr:uid="{A3F068D6-0D9F-534D-A11E-DAA612C3C742}"/>
-    <hyperlink ref="A21" r:id="rId175" display="https://ecos.fws.gov/ecp/species/7798" xr:uid="{D93E9E4F-BBEB-6E4F-B627-B82EFAD20987}"/>
-    <hyperlink ref="A24" r:id="rId176" display="https://ecos.fws.gov/ecp/species/1300" xr:uid="{96AEE1F4-A18E-2341-B553-7FD082C12021}"/>
-    <hyperlink ref="A25" r:id="rId177" display="https://ecos.fws.gov/ecp/species/6679" xr:uid="{8AB70AC6-7481-6F4F-9EE4-2442283B23F6}"/>
-    <hyperlink ref="A26" r:id="rId178" display="https://ecos.fws.gov/ecp/species/7577" xr:uid="{BE789AC0-ADC4-FC45-9A0A-D2611684E51E}"/>
-    <hyperlink ref="A27" r:id="rId179" display="https://ecos.fws.gov/ecp/species/4807" xr:uid="{30119158-FE03-2649-B590-19D332FD0366}"/>
-    <hyperlink ref="A31" r:id="rId180" display="https://ecos.fws.gov/ecp/species/8125" xr:uid="{47D09E27-3439-CF4E-8EA5-3D7FCC0ED34C}"/>
-    <hyperlink ref="A32" r:id="rId181" display="https://ecos.fws.gov/ecp/species/5023" xr:uid="{C04191E6-C8C4-1642-9476-315C3B6E1406}"/>
-    <hyperlink ref="A33" r:id="rId182" display="https://ecos.fws.gov/ecp/species/1807" xr:uid="{1EBDEC32-9875-444A-A6EB-7881400C19A8}"/>
-    <hyperlink ref="A40" r:id="rId183" display="https://ecos.fws.gov/ecp/species/2285" xr:uid="{EB089F99-EB84-E54C-878F-94E15251CDEF}"/>
-    <hyperlink ref="A41" r:id="rId184" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=Q3P5" xr:uid="{085784BB-41F9-4E42-AC37-2AE37811F7ED}"/>
-    <hyperlink ref="A68" r:id="rId185" display="https://ecos.fws.gov/ecp/species/8963" xr:uid="{4E9A384E-3163-554E-9555-6A3C9EE328D2}"/>
-    <hyperlink ref="A72" r:id="rId186" display="https://ecos.fws.gov/ecp/species/8619" xr:uid="{FA916CD7-E9ED-2541-936D-5F891F6E94C6}"/>
-    <hyperlink ref="A47" r:id="rId187" display="https://ecos.fws.gov/ecp/species/9627" xr:uid="{06BADA9A-0F87-814D-81E1-2AF6E641F8E4}"/>
-    <hyperlink ref="A87" r:id="rId188" display="https://ecos.fws.gov/ecp/species/8736" xr:uid="{961A49D4-4271-D54C-A7E3-EF7724CB70A6}"/>
-    <hyperlink ref="A92" r:id="rId189" display="https://ecos.fws.gov/ecp/species/2375" xr:uid="{BEECF353-AE88-7947-AB0C-0C77A17D71E5}"/>
-    <hyperlink ref="A94" r:id="rId190" display="https://ecos.fws.gov/ecp/species/9927" xr:uid="{0F949A64-0A3C-D540-9FD9-EF8EAED13F68}"/>
-    <hyperlink ref="A95" r:id="rId191" display="https://ecos.fws.gov/ecp/species/9929" xr:uid="{890A6171-C275-AC47-AEC8-EB04860B1DE3}"/>
-    <hyperlink ref="A97" r:id="rId192" display="https://ecos.fws.gov/ecp/species/2841" xr:uid="{557863FF-6902-1049-89D2-CE513BF2E5A4}"/>
-    <hyperlink ref="A98" r:id="rId193" display="https://ecos.fws.gov/ecp/species/5825" xr:uid="{641A797C-6175-6F45-9CDA-01C14FDCCFCC}"/>
-    <hyperlink ref="A130" r:id="rId194" display="https://ecos.fws.gov/ecp/species/572" xr:uid="{D672B3F0-29D4-0C48-8327-D0ADF4AFC538}"/>
-    <hyperlink ref="A134" r:id="rId195" display="https://ecos.fws.gov/ecp/species/8382" xr:uid="{5728097E-CC3A-4F4A-9C68-5D0967385602}"/>
-    <hyperlink ref="A142" r:id="rId196" display="https://ecos.fws.gov/ecp/species/9933" xr:uid="{4D799BB5-0AC6-7746-8FDC-FACE634842CB}"/>
-    <hyperlink ref="A148" r:id="rId197" display="https://ecos.fws.gov/ecp/species/3833" xr:uid="{570A4D50-B04C-364F-A754-EC5C1FB7F83E}"/>
-    <hyperlink ref="A156" r:id="rId198" display="https://ecos.fws.gov/ecp/species/2378" xr:uid="{BC916449-17EF-DB41-ABC8-329B8F308A53}"/>
-    <hyperlink ref="A158" r:id="rId199" display="https://ecos.fws.gov/ecp/species/7683" xr:uid="{EF8AA05B-1D2F-AA4E-A33E-5536D0965255}"/>
-    <hyperlink ref="A167" r:id="rId200" display="https://ecos.fws.gov/ecp/species/279" xr:uid="{A5133E10-E45E-BA42-9BAE-8D3E3E17A48B}"/>
-    <hyperlink ref="A170" r:id="rId201" display="https://ecos.fws.gov/ecp/species/879" xr:uid="{52D06944-1626-3C43-BAFC-BEC4831AA5DB}"/>
-    <hyperlink ref="A176" r:id="rId202" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=Q2UP" xr:uid="{FDC6F224-EBF2-054F-AD01-BBFEFD85F731}"/>
-    <hyperlink ref="A182" r:id="rId203" display="https://ecos.fws.gov/ecp/species/3325" xr:uid="{5E2D827F-E163-2A44-8A32-562FA0DF5E23}"/>
-    <hyperlink ref="A196" r:id="rId204" display="https://ecos.fws.gov/ecp/species/9937" xr:uid="{57BE5B8A-2933-CF46-B7E8-C6269AD67EB8}"/>
-    <hyperlink ref="A211" r:id="rId205" display="https://ecos.fws.gov/ecp/species/6441" xr:uid="{4B66B831-54A4-C84D-97D3-746E534A1DA0}"/>
-    <hyperlink ref="A212" r:id="rId206" display="https://ecos.fws.gov/ecp/species/1348" xr:uid="{C94B322B-07EC-8044-AB12-7215C57DFFD0}"/>
-    <hyperlink ref="A213" r:id="rId207" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=Q3F2" xr:uid="{BAD8198E-81E6-4A4D-8466-3CDAE0203BE5}"/>
-    <hyperlink ref="A220" r:id="rId208" display="https://ecos.fws.gov/ecp/species/599" xr:uid="{29C4D3A7-9631-9C46-BC35-5E2B52F190C7}"/>
-    <hyperlink ref="A224" r:id="rId209" display="https://ecos.fws.gov/ecp/species/1748" xr:uid="{B3C2191A-0069-624E-8D91-880CE56E1E6D}"/>
-    <hyperlink ref="A312" r:id="rId210" display="https://ecos.fws.gov/ecp/species/8397" xr:uid="{EBCD1C11-392F-234B-AA3D-D64983180592}"/>
-    <hyperlink ref="A314" r:id="rId211" display="https://ecos.fws.gov/ecp/species/883" xr:uid="{A649374D-E3C9-214A-BCB8-F8CC458D100D}"/>
-    <hyperlink ref="A315" r:id="rId212" display="https://ecos.fws.gov/ecp/species/6796" xr:uid="{13F55EB7-C340-8745-89A7-02B6DA3CADFA}"/>
-    <hyperlink ref="A318" r:id="rId213" display="https://ecos.fws.gov/ecp/species/5588" xr:uid="{D6509748-8754-734A-8E23-315B55C63B2B}"/>
-    <hyperlink ref="A319" r:id="rId214" display="https://ecos.fws.gov/ecp/species/2227" xr:uid="{70627C4D-4065-7542-B7AF-A55FF597F299}"/>
-    <hyperlink ref="A329" r:id="rId215" display="https://ecos.fws.gov/ecp/species/3157" xr:uid="{8046201C-7F62-CD41-89CB-270425083D64}"/>
-    <hyperlink ref="A331" r:id="rId216" display="https://ecos.fws.gov/ecp/species/2856" xr:uid="{E7DE1317-C80C-6C44-9A49-F6F8F346EDA5}"/>
-    <hyperlink ref="A345" r:id="rId217" display="https://ecos.fws.gov/ecp/species/9029" xr:uid="{5C6A3194-DD79-3445-841B-FDC7A54EDB20}"/>
-    <hyperlink ref="A361" r:id="rId218" display="https://ecos.fws.gov/ecp/species/1848" xr:uid="{D7815388-0B25-DF4F-B284-4869D133A980}"/>
-    <hyperlink ref="A2" r:id="rId219" display="https://ecos.fws.gov/ecp/species/9914" xr:uid="{A7A8C81D-056E-9B4B-8E64-EAE14931388A}"/>
-    <hyperlink ref="A20" r:id="rId220" display="https://ecos.fws.gov/ecp/species/9141" xr:uid="{250B8AB4-08B0-EC4B-A5B2-2EEFCF37120F}"/>
-    <hyperlink ref="A28" r:id="rId221" display="https://ecos.fws.gov/ecp/species/8601" xr:uid="{080E1ED8-C529-464D-AFD1-B04E3AA126FE}"/>
-    <hyperlink ref="A29" r:id="rId222" display="https://ecos.fws.gov/ecp/species/9005" xr:uid="{2CC35D3C-B66D-9A42-912F-6B32580E6422}"/>
-    <hyperlink ref="A30" r:id="rId223" display="https://ecos.fws.gov/ecp/species/8270" xr:uid="{E21D9869-7AB0-5A41-9B30-04202DF00EE2}"/>
-    <hyperlink ref="A42" r:id="rId224" display="https://ecos.fws.gov/ecp/species/7022" xr:uid="{EC4ABD3A-5CD9-9249-9AB4-FE6E936A3F4E}"/>
-    <hyperlink ref="A44" r:id="rId225" display="https://ecos.fws.gov/ecp/species/10403" xr:uid="{E1F7BC20-0ECC-0D4F-9C30-31FF11E7C55C}"/>
-    <hyperlink ref="A66" r:id="rId226" display="https://ecos.fws.gov/ecp/species/8134" xr:uid="{E8B8C5A0-5B0F-9C44-B6A3-51A16B942EA1}"/>
-    <hyperlink ref="A67" r:id="rId227" display="https://ecos.fws.gov/ecp/species/9982" xr:uid="{2B1635C7-02F3-1344-B67F-5A9340CD6BDC}"/>
-    <hyperlink ref="A71" r:id="rId228" display="https://ecos.fws.gov/ecp/species/9053" xr:uid="{60700EB9-3856-B34E-877C-64D025ABDA49}"/>
-    <hyperlink ref="A81" r:id="rId229" display="https://ecos.fws.gov/ecp/species/9743" xr:uid="{A05FC1A8-19BB-ED4E-AA32-50F3B9D608F7}"/>
-    <hyperlink ref="A108" r:id="rId230" display="https://ecos.fws.gov/ecp/species/3285" xr:uid="{0237321C-939C-DC48-9D5B-498BE5D56A8D}"/>
-    <hyperlink ref="A111" r:id="rId231" display="https://ecos.fws.gov/ecp/species/9209" xr:uid="{4833C1BB-1050-0D4E-A21F-725D719C97F8}"/>
-    <hyperlink ref="A112" r:id="rId232" display="https://ecos.fws.gov/ecp/species/9208" xr:uid="{8129E995-3DB7-3F42-B602-EFB261DF1067}"/>
-    <hyperlink ref="A113" r:id="rId233" display="https://ecos.fws.gov/ecp/species/9779" xr:uid="{5BF7124A-71C1-B345-835F-8B9E48B7DDC3}"/>
-    <hyperlink ref="A114" r:id="rId234" display="https://ecos.fws.gov/ecp/species/9781" xr:uid="{E0E7C544-F570-0348-82AD-7D52CE929A08}"/>
-    <hyperlink ref="A140" r:id="rId235" display="https://ecos.fws.gov/ecp/species/5618" xr:uid="{873F2B97-CACF-B84E-B745-E87604F1B592}"/>
-    <hyperlink ref="A146" r:id="rId236" display="https://ecos.fws.gov/ecp/species/8768" xr:uid="{DB10DE9D-21BA-474A-905F-6003EC0088F9}"/>
-    <hyperlink ref="A155" r:id="rId237" display="https://ecos.fws.gov/ecp/species/5640" xr:uid="{DB718CDE-F7B5-B740-9C37-F7FA50FB58C6}"/>
-    <hyperlink ref="A173" r:id="rId238" display="https://ecos.fws.gov/ecp/species/8852" xr:uid="{BA298C64-9585-FF4C-B230-7677A828FFA6}"/>
-    <hyperlink ref="A174" r:id="rId239" display="https://ecos.fws.gov/ecp/species/8602" xr:uid="{E747DA66-A794-AC40-9460-47C328CA02E2}"/>
-    <hyperlink ref="A175" r:id="rId240" display="https://ecos.fws.gov/ecp/species/4379" xr:uid="{9ABB73AE-4990-AC43-B625-F7F7577E0A39}"/>
-    <hyperlink ref="A184" r:id="rId241" display="https://ecos.fws.gov/ecp/species/6613" xr:uid="{4BCD9FF3-13F7-EF44-8585-CD3860F30541}"/>
-    <hyperlink ref="A201" r:id="rId242" display="https://ecos.fws.gov/ecp/species/3057" xr:uid="{0FE754B7-4B8D-0046-A5CF-A932B60510AD}"/>
-    <hyperlink ref="A210" r:id="rId243" display="https://ecos.fws.gov/ecp/species/7863" xr:uid="{5F6B341E-4C77-D74C-BDA8-00E3B7C0913D}"/>
-    <hyperlink ref="A248" r:id="rId244" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=I0J3" xr:uid="{90801182-17AC-FE41-BCC7-988F7E617A17}"/>
-    <hyperlink ref="A249" r:id="rId245" display="https://ecos.fws.gov/ecp/species/6127" xr:uid="{3D8F9A2A-C5E6-8C40-9A3E-A3B4E4B73488}"/>
-    <hyperlink ref="A250" r:id="rId246" display="https://ecos.fws.gov/ecp/species/2819" xr:uid="{EEEB47C7-85F6-E540-B47B-6921201DB40B}"/>
-    <hyperlink ref="A251" r:id="rId247" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=I0JH" xr:uid="{5810F599-D671-5849-A592-9913575BD4CC}"/>
-    <hyperlink ref="A252" r:id="rId248" display="https://ecos.fws.gov/ecp/species/6531" xr:uid="{6A27090F-899D-F24B-9052-3324BA73EB7B}"/>
-    <hyperlink ref="A253" r:id="rId249" display="https://ecos.fws.gov/ecp/species/1411" xr:uid="{4E00BB03-A026-8C4F-8AC1-13F5A5434DCD}"/>
-    <hyperlink ref="A254" r:id="rId250" display="https://ecos.fws.gov/ecp/species/3401" xr:uid="{42ABB0C5-55E3-5A43-BA11-9255629917A1}"/>
-    <hyperlink ref="A255" r:id="rId251" display="https://ecos.fws.gov/ecp/species/6128" xr:uid="{5D956EE9-D9E5-1D49-88D5-4EA884B01BD9}"/>
-    <hyperlink ref="A256" r:id="rId252" display="https://ecos.fws.gov/ecp/species/6075" xr:uid="{E66E3689-F6B9-084C-BD2D-423923BEE121}"/>
-    <hyperlink ref="A257" r:id="rId253" display="https://ecos.fws.gov/ecp/species/3142" xr:uid="{1FB67122-101D-724A-B599-33EC6127AB47}"/>
-    <hyperlink ref="A258" r:id="rId254" display="https://ecos.fws.gov/ecp/species/8016" xr:uid="{4AA23102-D4D0-B744-B7B7-9C01C235B996}"/>
-    <hyperlink ref="A259" r:id="rId255" display="https://ecos.fws.gov/ecp/species/8223" xr:uid="{26374774-4461-454F-A511-0A216584F004}"/>
-    <hyperlink ref="A260" r:id="rId256" display="https://ecos.fws.gov/ecp/species/1791" xr:uid="{432BE856-44B7-6540-832F-E8E962B272ED}"/>
-    <hyperlink ref="A261" r:id="rId257" display="https://ecos.fws.gov/ecp/species/7174" xr:uid="{97EA6E83-6060-8E45-A4EB-CBAFB0D1FDA4}"/>
-    <hyperlink ref="A262" r:id="rId258" display="https://ecos.fws.gov/ecp/species/8537" xr:uid="{E0A10225-0CEE-034F-AC4A-13628805ADF7}"/>
-    <hyperlink ref="A263" r:id="rId259" display="https://ecos.fws.gov/ecp/species/5059" xr:uid="{65C791CD-5C49-734F-B334-616228F2935B}"/>
-    <hyperlink ref="A264" r:id="rId260" display="https://ecos.fws.gov/ecp/species/7025" xr:uid="{6E3A68D4-5C44-0044-BC46-A70348A69CCC}"/>
-    <hyperlink ref="A265" r:id="rId261" display="https://ecos.fws.gov/ecp/species/5654" xr:uid="{B1A49F6A-2F10-F84B-B451-A4546A238067}"/>
-    <hyperlink ref="A308" r:id="rId262" display="https://ecos.fws.gov/ecp/species/9869" xr:uid="{22E1137B-5F2A-8E4E-B3F5-CC3566EB25A1}"/>
-    <hyperlink ref="A309" r:id="rId263" display="https://ecos.fws.gov/ecp/species/218" xr:uid="{5A1DDA99-40E0-F342-AF7F-2CA489CDEA8B}"/>
-    <hyperlink ref="A320" r:id="rId264" display="https://ecos.fws.gov/ecp/species/7553" xr:uid="{5C24E9C7-0708-074F-8B69-86188E79D7D5}"/>
-    <hyperlink ref="A325" r:id="rId265" display="https://ecos.fws.gov/ecp/species/8145" xr:uid="{29F1D7EF-F1B0-5446-A0E5-F44C70387EAA}"/>
-    <hyperlink ref="A326" r:id="rId266" display="https://ecos.fws.gov/ecp/species/2813" xr:uid="{1D55CFD7-98A4-8C4C-A051-ADAE1DF78334}"/>
-    <hyperlink ref="A339" r:id="rId267" display="https://ecos.fws.gov/ecp/species/9924" xr:uid="{F9F8FDEC-2856-DF47-8ADF-95AE578B0DB8}"/>
-    <hyperlink ref="A19" r:id="rId268" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=A0J3" xr:uid="{9FCD13C7-987A-D949-B48A-6D79074E5C25}"/>
-    <hyperlink ref="A77" r:id="rId269" display="https://ecos.fws.gov/ecp/species/7401" xr:uid="{0F1BEB22-6A53-F044-AFB9-50F72D858F56}"/>
-    <hyperlink ref="A85" r:id="rId270" display="https://ecos.fws.gov/ecp/species/2985" xr:uid="{75786265-65B3-BB49-8FA6-1A7399ACAB86}"/>
-    <hyperlink ref="A136" r:id="rId271" display="https://ecos.fws.gov/ecp/species/5123" xr:uid="{FD5FED9D-31FC-684C-B13D-7D769F82ABBB}"/>
-    <hyperlink ref="A179" r:id="rId272" display="https://ecos.fws.gov/ecp/species/3651" xr:uid="{433D049B-B6D4-5842-83EA-B5D564DFB021}"/>
-    <hyperlink ref="A185" r:id="rId273" display="https://ecos.fws.gov/ecp/species/9051" xr:uid="{F3A8D873-9F74-8A4D-8EC2-1FE366D9B4E0}"/>
-    <hyperlink ref="A199" r:id="rId274" display="https://ecos.fws.gov/ecp/species/8791" xr:uid="{DA852D23-8E67-384A-9BD7-2732CBC6F45B}"/>
-    <hyperlink ref="A327" r:id="rId275" display="https://ecos.fws.gov/ecp/species/2984" xr:uid="{EC605DE9-D94C-034D-BE0F-12435E45F89B}"/>
-    <hyperlink ref="A340" r:id="rId276" display="https://ecos.fws.gov/ecp/species/5126" xr:uid="{AD56C8A9-43E9-DE45-9FE4-695D1AAB2D76}"/>
-    <hyperlink ref="A363" r:id="rId277" display="https://ecos.fws.gov/ecp/species/4252" xr:uid="{2AB82B5D-CBA6-444F-A35C-5C7B3A732A32}"/>
-    <hyperlink ref="A181" r:id="rId278" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=S02V" xr:uid="{B2D70AAF-A561-8B46-ADBC-3512B3A130B4}"/>
-    <hyperlink ref="A227" r:id="rId279" display="https://ecos.fws.gov/ecp/species/8100" xr:uid="{E8057E05-FB62-FA47-8784-979385D8981C}"/>
-    <hyperlink ref="A3" r:id="rId280" display="https://ecos.fws.gov/ecp/species/1833" xr:uid="{63A9D92A-E637-FC41-A5C4-C48CFBE5341C}"/>
-    <hyperlink ref="A22" r:id="rId281" display="https://ecos.fws.gov/ecp/species/8793" xr:uid="{C06B57C4-A1F3-574F-9B5D-E7ECF80F6014}"/>
-    <hyperlink ref="A64" r:id="rId282" display="https://ecos.fws.gov/ecp/species/3525" xr:uid="{58D710FD-1276-1B4F-9FFC-555FFC4FC942}"/>
-    <hyperlink ref="A70" r:id="rId283" display="https://ecos.fws.gov/ecp/species/4979" xr:uid="{090965A1-13D4-5942-A72D-95754AECA1A4}"/>
-    <hyperlink ref="A82" r:id="rId284" display="https://ecos.fws.gov/ecp/species/9903" xr:uid="{1760FEB8-C0A4-4544-B969-827C32C37499}"/>
-    <hyperlink ref="A84" r:id="rId285" display="https://ecos.fws.gov/ecp/species/6768" xr:uid="{15B7D83E-9237-D24F-8C24-899F7A4405A9}"/>
-    <hyperlink ref="A89" r:id="rId286" display="https://ecos.fws.gov/ecp/species/47" xr:uid="{4C8B457F-ECC3-8649-B838-9AFF1812ACAE}"/>
-    <hyperlink ref="A93" r:id="rId287" display="https://ecos.fws.gov/ecp/species/6056" xr:uid="{87815E7C-C47F-734B-B3CB-371329D3D8FE}"/>
-    <hyperlink ref="A109" r:id="rId288" display="https://ecos.fws.gov/ecp/species/4480" xr:uid="{0A9A51F2-0791-C242-B88F-2CFCF4F7F700}"/>
-    <hyperlink ref="A110" r:id="rId289" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=C050" xr:uid="{C3CD780A-497A-9D43-A4E5-91CC8169047F}"/>
-    <hyperlink ref="A131" r:id="rId290" display="https://ecos.fws.gov/ecp/species/6997" xr:uid="{9FD2F6F8-D3E1-D548-B92A-2DE68426B6A3}"/>
-    <hyperlink ref="A132" r:id="rId291" display="https://ecos.fws.gov/ecp/species/6994" xr:uid="{C9FD3986-569A-AC4C-8192-2A2201FDDEF1}"/>
-    <hyperlink ref="A133" r:id="rId292" display="https://ecos.fws.gov/ecp/species/3085" xr:uid="{4E41431E-D574-A243-AB6C-95BDC760D6AB}"/>
-    <hyperlink ref="A147" r:id="rId293" display="https://ecos.fws.gov/ecp/species/3248" xr:uid="{8B63A8A7-6BA6-D445-B7D0-CF7E8DA3C724}"/>
-    <hyperlink ref="A152" r:id="rId294" display="https://ecos.fws.gov/ecp/species/9044" xr:uid="{6027797E-5D96-BA4B-B225-8BF7990F2BF0}"/>
-    <hyperlink ref="A178" r:id="rId295" display="https://ecos.fws.gov/ecp/species/4658" xr:uid="{998C2B89-AC49-8D42-B490-0188A82A89E0}"/>
-    <hyperlink ref="A226" r:id="rId296" display="https://ecos.fws.gov/ecp/species/4978" xr:uid="{DE885E6C-C66F-E549-ACC0-8839B33A5818}"/>
-    <hyperlink ref="A267" r:id="rId297" display="https://ecos.fws.gov/ecp/species/9957" xr:uid="{89C6D7CC-174C-D04E-9F56-2AE08A646C10}"/>
-    <hyperlink ref="A317" r:id="rId298" display="https://ecos.fws.gov/ecp/species/9087" xr:uid="{5E752F79-2715-8943-814B-53E97A27F8DE}"/>
-    <hyperlink ref="A330" r:id="rId299" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=C07C" xr:uid="{B794AB29-7FDC-C44D-921D-0492B07800AA}"/>
-    <hyperlink ref="A341" r:id="rId300" display="https://ecos.fws.gov/ecp/species/1497" xr:uid="{9748C32F-9C8D-2145-BB52-2B28630A320F}"/>
-    <hyperlink ref="A75" r:id="rId301" display="https://ecos.fws.gov/ecp/species/294" xr:uid="{4997B699-FEFB-2243-AF81-C1838D2B55CD}"/>
-    <hyperlink ref="A76" r:id="rId302" display="https://ecos.fws.gov/ecp/species/8598" xr:uid="{F88EA5DA-6E14-B94A-8ED1-49EDA381ACC2}"/>
-    <hyperlink ref="A83" r:id="rId303" display="https://ecos.fws.gov/ecp/species/8642" xr:uid="{1833321D-A53C-264B-83A0-A5D48C450F84}"/>
-    <hyperlink ref="A90" r:id="rId304" display="https://ecos.fws.gov/ecp/species/9896" xr:uid="{D06B3CB6-BF50-8048-9351-C7BDC1F36794}"/>
-    <hyperlink ref="A145" r:id="rId305" display="https://ecos.fws.gov/ecp/species/8641" xr:uid="{4B9F62CF-D1B9-DA49-AAD2-9E6A4F025A79}"/>
-    <hyperlink ref="A169" r:id="rId306" display="https://ecos.fws.gov/ecp/species/9911" xr:uid="{7ABF6ED7-BDE7-0247-B9C7-20C92D8F63C2}"/>
-    <hyperlink ref="A183" r:id="rId307" display="https://ecos.fws.gov/ecp/species/4369" xr:uid="{5F1EBB6A-AA1F-5145-BA40-FBD8E49A96ED}"/>
-    <hyperlink ref="A209" r:id="rId308" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=G0EB" xr:uid="{773F7FBA-0F90-4645-B8C6-3C012182D921}"/>
-    <hyperlink ref="A221" r:id="rId309" display="https://ecos.fws.gov/ecp/species/7006" xr:uid="{50B3DD9B-EAEB-3349-84FB-0AF848F3F20F}"/>
-    <hyperlink ref="A228" r:id="rId310" display="https://ecos.fws.gov/ecp/species/6216" xr:uid="{9730A146-ED06-2945-A97C-E5D0F28699EA}"/>
-    <hyperlink ref="A270" r:id="rId311" display="https://ecos.fws.gov/ecp/species/4987" xr:uid="{45CCE743-EB0E-EA4D-8F86-3FDAE65F5E28}"/>
-    <hyperlink ref="A271" r:id="rId312" display="https://ecos.fws.gov/ecp/species/8978" xr:uid="{5A4CCFF5-7CC1-054F-A702-FEB18266A8B4}"/>
-    <hyperlink ref="A272" r:id="rId313" display="https://ecos.fws.gov/ecp/species/8979" xr:uid="{33263263-43E6-7F42-8BFA-4ED660757361}"/>
-    <hyperlink ref="A273" r:id="rId314" display="https://ecos.fws.gov/ecp/species/9913" xr:uid="{A501B99B-BE81-F741-85EC-E7253F89E413}"/>
-    <hyperlink ref="A274" r:id="rId315" display="https://ecos.fws.gov/ecp/species/8980" xr:uid="{7BA54CAF-17CC-4C4F-97D0-2D292EDCF695}"/>
-    <hyperlink ref="A275" r:id="rId316" display="https://ecos.fws.gov/ecp/species/4830" xr:uid="{4E5E779F-CF5D-F240-A459-C8504FE32B7D}"/>
-    <hyperlink ref="A276" r:id="rId317" display="https://ecos.fws.gov/ecp/species/8981" xr:uid="{A88140F5-20E6-1B49-A5CD-40BFD2AA9ACC}"/>
-    <hyperlink ref="A277" r:id="rId318" display="https://ecos.fws.gov/ecp/species/7545" xr:uid="{86E13FCB-E819-534E-AC7A-904CB81463F2}"/>
-    <hyperlink ref="A278" r:id="rId319" display="https://ecos.fws.gov/ecp/species/1399" xr:uid="{FFB68022-6D9D-4241-B712-CE30B0F26D02}"/>
-    <hyperlink ref="A279" r:id="rId320" display="https://ecos.fws.gov/ecp/species/8982" xr:uid="{B9010237-DB8E-1F4C-BB10-986E55F870B8}"/>
-    <hyperlink ref="A281" r:id="rId321" display="https://ecos.fws.gov/ecp/species/8985" xr:uid="{91F0E7F3-3706-DF45-9A43-EBAB7360A45B}"/>
-    <hyperlink ref="A282" r:id="rId322" display="https://ecos.fws.gov/ecp/species/1380" xr:uid="{CCBE3125-7253-FE4E-9710-731F17350D8E}"/>
-    <hyperlink ref="A284" r:id="rId323" display="https://ecos.fws.gov/ecp/species/8987" xr:uid="{8DAB7C63-A47B-184C-AA21-D8C1546BDBBF}"/>
-    <hyperlink ref="A285" r:id="rId324" display="https://ecos.fws.gov/ecp/species/8989" xr:uid="{15C90215-F1E3-2D4C-8EF6-2250991B556B}"/>
-    <hyperlink ref="A286" r:id="rId325" display="https://ecos.fws.gov/ecp/species/4778" xr:uid="{A59CDD50-28BF-FC4E-8296-9ABF8E70B868}"/>
-    <hyperlink ref="A287" r:id="rId326" display="https://ecos.fws.gov/ecp/species/5868" xr:uid="{548937D9-B0E1-E948-A300-3187CB9380CE}"/>
-    <hyperlink ref="A291" r:id="rId327" display="https://ecos.fws.gov/ecp/species/8994" xr:uid="{31B494FE-14D6-B542-8562-B692EEE42EEC}"/>
-    <hyperlink ref="A294" r:id="rId328" display="https://ecos.fws.gov/ecp/species/8996" xr:uid="{03C32A2F-A893-5E49-B35D-3B060D992EE9}"/>
-    <hyperlink ref="A298" r:id="rId329" display="https://ecos.fws.gov/ecp/species/9000" xr:uid="{7AB68529-EA6D-B54B-B2B9-9002B1897920}"/>
-    <hyperlink ref="A321" r:id="rId330" display="https://ecos.fws.gov/ecp/species/1015" xr:uid="{3DA46EB9-EFA1-A346-A3A0-BB03A6121C1B}"/>
-    <hyperlink ref="A322" r:id="rId331" display="https://ecos.fws.gov/ecp/species/7840" xr:uid="{4B10B1E8-9209-8D4C-BAD2-CC9CCE215434}"/>
-    <hyperlink ref="A323" r:id="rId332" display="https://ecos.fws.gov/ecp/species/4377" xr:uid="{735B4EDF-A337-AD40-94B5-0EC887206D30}"/>
-    <hyperlink ref="A346" r:id="rId333" display="https://ecos.fws.gov/ecp/species/8849" xr:uid="{A22843EF-9822-8640-B572-BF13BEA9CEF0}"/>
-    <hyperlink ref="A350" r:id="rId334" display="https://ecos.fws.gov/ecp/species/6645" xr:uid="{AB3ED14A-8398-8340-8DDF-4CB07D95CC2B}"/>
-    <hyperlink ref="A351" r:id="rId335" display="https://ecos.fws.gov/ecp/species/303" xr:uid="{09E6B8E2-F3DA-A249-8845-6241DDE97B65}"/>
-    <hyperlink ref="A352" r:id="rId336" display="https://ecos.fws.gov/ecp/species/7837" xr:uid="{323C5521-385F-3749-BD80-9C796736583E}"/>
-    <hyperlink ref="A353" r:id="rId337" display="https://ecos.fws.gov/ecp/species/2556" xr:uid="{E65B2E6A-16DB-9049-A799-DE3605A1D06F}"/>
-    <hyperlink ref="A354" r:id="rId338" display="https://ecos.fws.gov/ecp/species/4521" xr:uid="{A27A40CA-50B3-9445-A36B-D2170709F07C}"/>
-    <hyperlink ref="A355" r:id="rId339" display="https://ecos.fws.gov/ecp/species/6906" xr:uid="{D435C3D7-C2FD-094D-8B5A-6F242AD663F0}"/>
-    <hyperlink ref="A358" r:id="rId340" display="https://ecos.fws.gov/ecp/species/8761" xr:uid="{A4D83D16-B766-1648-AABF-2621C8BF7767}"/>
-    <hyperlink ref="A359" r:id="rId341" display="https://ecos.fws.gov/ecp/species/8850" xr:uid="{931D2621-747D-1249-9F78-6506CAA2814A}"/>
-    <hyperlink ref="A360" r:id="rId342" display="https://ecos.fws.gov/ecp/species/8896" xr:uid="{44846242-77B0-2244-B039-0F1F776F32F1}"/>
+    <hyperlink ref="A267" r:id="rId42" display="https://ecos.fws.gov/ecp/species/4748" xr:uid="{D6A80F96-E67C-9248-8B93-DB514A0AA157}"/>
+    <hyperlink ref="A331" r:id="rId43" display="https://ecos.fws.gov/ecp/species/1123" xr:uid="{2327E9D8-03CC-D444-B3D9-9A258367AFA5}"/>
+    <hyperlink ref="A332" r:id="rId44" display="https://ecos.fws.gov/ecp/species/7266" xr:uid="{58F3BDC2-A1C9-C043-8806-EE9B241A1797}"/>
+    <hyperlink ref="A355" r:id="rId45" display="https://ecos.fws.gov/ecp/species/1924" xr:uid="{E9C68340-A8B5-6D4B-B843-B2CC10A96B1A}"/>
+    <hyperlink ref="A356" r:id="rId46" display="https://ecos.fws.gov/ecp/species/8745" xr:uid="{BAA30E52-B6D7-9942-9537-6242538ACB3C}"/>
+    <hyperlink ref="A7" r:id="rId47" display="https://ecos.fws.gov/ecp/species/9871" xr:uid="{3CAF6253-BEDA-2B4E-AB77-3CB3F288456E}"/>
+    <hyperlink ref="A8" r:id="rId48" display="https://ecos.fws.gov/ecp/species/785" xr:uid="{9B415958-C9C0-7E47-9ED4-69DCEA8ED60B}"/>
+    <hyperlink ref="A18" r:id="rId49" display="https://ecos.fws.gov/ecp/species/9873" xr:uid="{8A41C26E-EB2E-6D46-9037-07B8CDA71829}"/>
+    <hyperlink ref="A80" r:id="rId50" display="https://ecos.fws.gov/ecp/species/6895" xr:uid="{5D628A9F-F97A-6D4F-80C8-0E2B6A3E0966}"/>
+    <hyperlink ref="A235" r:id="rId51" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=F04A" xr:uid="{0C77E00D-7479-2546-92D1-E8848E5AA481}"/>
+    <hyperlink ref="A91" r:id="rId52" display="https://ecos.fws.gov/ecp/species/4511" xr:uid="{4E13999E-400D-3747-889F-EA2EB7DD1966}"/>
+    <hyperlink ref="A126" r:id="rId53" display="https://ecos.fws.gov/ecp/species/10339" xr:uid="{233FCAF0-5E24-4D4D-B962-A75DE9ECE53E}"/>
+    <hyperlink ref="A127" r:id="rId54" display="https://ecos.fws.gov/ecp/species/5164" xr:uid="{851A08BA-1420-F04F-A6DA-04EB37A7885C}"/>
+    <hyperlink ref="A128" r:id="rId55" display="https://ecos.fws.gov/ecp/species/9880" xr:uid="{35FB8694-887A-3B43-BC8D-B66E2DD9D878}"/>
+    <hyperlink ref="A161" r:id="rId56" display="https://ecos.fws.gov/ecp/species/9041" xr:uid="{7B59DEF7-F228-8C4F-AAD2-5882E9C1D5B0}"/>
+    <hyperlink ref="A162" r:id="rId57" display="https://ecos.fws.gov/ecp/species/7540" xr:uid="{7E64CC29-B338-C941-A539-6A27E0EDB847}"/>
+    <hyperlink ref="A163" r:id="rId58" display="https://ecos.fws.gov/ecp/species/783" xr:uid="{892C26C0-0086-CA45-8C07-EF4D32F6D475}"/>
+    <hyperlink ref="A164" r:id="rId59" display="https://ecos.fws.gov/ecp/species/7541" xr:uid="{0E357956-E3E5-9F45-9EBD-4D987C457F75}"/>
+    <hyperlink ref="A180" r:id="rId60" display="https://ecos.fws.gov/ecp/species/9881" xr:uid="{C79F7F02-2064-F34B-A701-ACFB26818322}"/>
+    <hyperlink ref="A197" r:id="rId61" display="https://ecos.fws.gov/ecp/species/9879" xr:uid="{61D6C1A0-2EB2-4942-A04D-4549011B7484}"/>
+    <hyperlink ref="A198" r:id="rId62" display="https://ecos.fws.gov/ecp/species/9883" xr:uid="{8D019D16-00BB-4445-8133-0215EF2A30BA}"/>
+    <hyperlink ref="A224" r:id="rId63" display="https://ecos.fws.gov/ecp/species/3533" xr:uid="{8D550F40-E620-FC4F-A68E-D94B4A821B3F}"/>
+    <hyperlink ref="A229" r:id="rId64" display="https://ecos.fws.gov/ecp/species/4693" xr:uid="{1D58E5BA-28A6-6F4D-B838-6498056FEBA7}"/>
+    <hyperlink ref="A230" r:id="rId65" display="https://ecos.fws.gov/ecp/species/3254" xr:uid="{02AAC49B-8BCC-4A4E-A34E-2102F63D1E29}"/>
+    <hyperlink ref="A231" r:id="rId66" display="https://ecos.fws.gov/ecp/species/10233" xr:uid="{FEADB3DB-0ED3-EA4A-8E3C-0A67707938AE}"/>
+    <hyperlink ref="A232" r:id="rId67" display="https://ecos.fws.gov/ecp/species/1937" xr:uid="{CDEC4061-FB93-F349-BBFE-7D736A2A8647}"/>
+    <hyperlink ref="A233" r:id="rId68" display="https://ecos.fws.gov/ecp/species/9887" xr:uid="{6D223629-DED1-9F44-A73D-2FAC5194E064}"/>
+    <hyperlink ref="A234" r:id="rId69" display="https://ecos.fws.gov/ecp/species/299" xr:uid="{F0074253-8EC8-BF46-AEEE-9CAA1371D397}"/>
+    <hyperlink ref="A268" r:id="rId70" display="https://ecos.fws.gov/ecp/species/8977" xr:uid="{BCB508DA-C3AC-F045-88C6-69AD75702B22}"/>
+    <hyperlink ref="A279" r:id="rId71" display="https://ecos.fws.gov/ecp/species/8984" xr:uid="{44F4B2A7-A544-264C-A1D2-BF046FF89B49}"/>
+    <hyperlink ref="A282" r:id="rId72" display="https://ecos.fws.gov/ecp/species/8986" xr:uid="{C834ECBB-37B9-1B42-86E5-9E3AAA949919}"/>
+    <hyperlink ref="A287" r:id="rId73" display="https://ecos.fws.gov/ecp/species/8991" xr:uid="{6B479769-5436-4B49-9A34-840C18BF88E6}"/>
+    <hyperlink ref="A288" r:id="rId74" display="https://ecos.fws.gov/ecp/species/8992" xr:uid="{E423C902-DC5D-E24E-BB1F-D7975BEAB797}"/>
+    <hyperlink ref="A289" r:id="rId75" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?sId=3974" xr:uid="{20E8A83E-8158-6B49-8D04-718FB5F66D83}"/>
+    <hyperlink ref="A291" r:id="rId76" display="https://ecos.fws.gov/ecp/species/2997" xr:uid="{5A1E9E5C-870C-EA49-80DF-8EC460C723C9}"/>
+    <hyperlink ref="A292" r:id="rId77" display="https://ecos.fws.gov/ecp/species/8995" xr:uid="{A117B146-3A81-D643-A5CD-47F117C9E584}"/>
+    <hyperlink ref="A294" r:id="rId78" display="https://ecos.fws.gov/ecp/species/8997" xr:uid="{11EF2442-A73B-6D4F-9FCA-2028DD48665C}"/>
+    <hyperlink ref="A295" r:id="rId79" display="https://ecos.fws.gov/ecp/species/8998" xr:uid="{1DF8CDE8-D5C5-6A4F-B635-25F3A3CA3AFC}"/>
+    <hyperlink ref="A296" r:id="rId80" display="https://ecos.fws.gov/ecp/species/8999" xr:uid="{DCD88F6A-67A1-6940-88D5-7CF452565E6B}"/>
+    <hyperlink ref="A298" r:id="rId81" display="https://ecos.fws.gov/ecp/species/9001" xr:uid="{9619CEDF-A496-A744-BF6A-AB1AC2BC9C63}"/>
+    <hyperlink ref="A299" r:id="rId82" display="https://ecos.fws.gov/ecp/species/9002" xr:uid="{36AE747F-A627-824A-9EB7-270C43E7661F}"/>
+    <hyperlink ref="A300" r:id="rId83" display="https://ecos.fws.gov/ecp/species/9042" xr:uid="{57C32620-21EF-4C4F-9D4A-B61AA95A8150}"/>
+    <hyperlink ref="A301" r:id="rId84" display="https://ecos.fws.gov/ecp/species/8967" xr:uid="{30D23C50-B8E2-7A45-BC14-26D58A4B9D17}"/>
+    <hyperlink ref="A302" r:id="rId85" display="https://ecos.fws.gov/ecp/species/8966" xr:uid="{A306EBCB-E2CE-E447-A8E1-97222AAD78E4}"/>
+    <hyperlink ref="A303" r:id="rId86" display="https://ecos.fws.gov/ecp/species/3963" xr:uid="{74BE6B4B-76AF-2E40-A138-2CC222EB1AC5}"/>
+    <hyperlink ref="A315" r:id="rId87" display="https://ecos.fws.gov/ecp/species/6208" xr:uid="{EED70E5B-9D26-2D49-90CA-118870A6E0FA}"/>
+    <hyperlink ref="A342" r:id="rId88" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?sId=8210" xr:uid="{DFED493E-EB40-5F46-AA73-A2E984E07853}"/>
+    <hyperlink ref="A343" r:id="rId89" display="https://ecos.fws.gov/ecp/species/7155" xr:uid="{1E34E677-E7C4-F249-A90C-2402FC5F8A34}"/>
+    <hyperlink ref="A347" r:id="rId90" display="https://ecos.fws.gov/ecp/species/7870" xr:uid="{93FABF54-3545-A24E-B617-EF15784A392A}"/>
+    <hyperlink ref="A348" r:id="rId91" display="https://ecos.fws.gov/ecp/species/8965" xr:uid="{0B5D3D0F-B248-D14F-A29E-7636E0459AF9}"/>
+    <hyperlink ref="A361" r:id="rId92" display="https://ecos.fws.gov/ecp/species/8209" xr:uid="{13123EB5-DF8F-0F42-A39E-E7A8A5B75CDB}"/>
+    <hyperlink ref="A46" r:id="rId93" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?sId=9860" xr:uid="{7C275CBF-8704-8E44-B8BA-4CEE7B08D9ED}"/>
+    <hyperlink ref="A49" r:id="rId94" display="https://ecos.fws.gov/ecp/species/9790" xr:uid="{72F112BE-6B1C-9742-B355-0718779B0AE5}"/>
+    <hyperlink ref="A50" r:id="rId95" display="https://ecos.fws.gov/ecp/species/9791" xr:uid="{451F3A23-F47B-1947-A485-1DC07C1E25E7}"/>
+    <hyperlink ref="A51" r:id="rId96" display="https://ecos.fws.gov/ecp/species/9792" xr:uid="{667508AB-7DA5-0F42-84A5-E7E671BDF9E1}"/>
+    <hyperlink ref="A52" r:id="rId97" display="https://ecos.fws.gov/ecp/species/9795" xr:uid="{9FC691A8-AF83-3645-B286-2447CDDC976A}"/>
+    <hyperlink ref="A53" r:id="rId98" display="https://ecos.fws.gov/ecp/species/4851" xr:uid="{7D9121C3-B9DD-8344-A871-9F8A31F2C592}"/>
+    <hyperlink ref="A54" r:id="rId99" display="https://ecos.fws.gov/ecp/species/9798" xr:uid="{28F1E893-3EE0-8D48-9848-69FAE8B37850}"/>
+    <hyperlink ref="A55" r:id="rId100" display="https://ecos.fws.gov/ecp/species/8539" xr:uid="{31A57676-4633-DA49-9DE6-C9D888CA1AA9}"/>
+    <hyperlink ref="A56" r:id="rId101" display="https://ecos.fws.gov/ecp/species/2605" xr:uid="{E5C360BB-492B-0D40-AFD6-07244CED5CF0}"/>
+    <hyperlink ref="A57" r:id="rId102" display="https://ecos.fws.gov/ecp/species/9801" xr:uid="{26D1E814-4F2E-4A40-8FA5-5EE500D86A2B}"/>
+    <hyperlink ref="A58" r:id="rId103" display="https://ecos.fws.gov/ecp/species/9803" xr:uid="{49020F91-2F3B-1B44-8495-FDDB64DD5320}"/>
+    <hyperlink ref="A61" r:id="rId104" display="https://ecos.fws.gov/ecp/species/9806" xr:uid="{7D04C721-CDFE-8943-80F0-247E98032568}"/>
+    <hyperlink ref="A121" r:id="rId105" display="https://ecos.fws.gov/ecp/species/5458" xr:uid="{D9C09780-CC8A-3C46-B019-49E73CEC5353}"/>
+    <hyperlink ref="A122" r:id="rId106" display="https://ecos.fws.gov/ecp/species/3289" xr:uid="{BCCE5561-28DB-BE4B-A2AB-DB1F9BAEE17F}"/>
+    <hyperlink ref="A149" r:id="rId107" display="https://ecos.fws.gov/ecp/species/9812" xr:uid="{6AB9325A-47DD-3941-9C6B-423985C60546}"/>
+    <hyperlink ref="A150" r:id="rId108" display="https://ecos.fws.gov/ecp/species/9813" xr:uid="{FB5C6046-E333-CF46-B1BF-6DFAD09111E6}"/>
+    <hyperlink ref="A151" r:id="rId109" display="https://ecos.fws.gov/ecp/species/9821" xr:uid="{8DB52BEB-8CD8-EC4B-9FA0-9BFE61257268}"/>
+    <hyperlink ref="A172" r:id="rId110" display="https://ecos.fws.gov/ecp/species/2692" xr:uid="{AB12A771-75D0-4848-AD27-F9A5AD5E3378}"/>
+    <hyperlink ref="A202" r:id="rId111" display="https://ecos.fws.gov/ecp/species/9815" xr:uid="{6984288D-6B1B-894D-A154-02CFF6FA93B9}"/>
+    <hyperlink ref="A203" r:id="rId112" display="https://ecos.fws.gov/ecp/species/9816" xr:uid="{AF88B8E7-4B6D-034A-9430-EBD6C1800EDF}"/>
+    <hyperlink ref="A204" r:id="rId113" display="https://ecos.fws.gov/ecp/species/9823" xr:uid="{4DFF5E55-762E-E844-BE02-9383D709EFBF}"/>
+    <hyperlink ref="A207" r:id="rId114" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=K07Q" xr:uid="{90CCD8F2-03C3-B741-AF81-F1AF45C9FC57}"/>
+    <hyperlink ref="A208" r:id="rId115" display="https://ecos.fws.gov/ecp/species/8226" xr:uid="{0EFD34B4-77C5-AA49-9CC3-4BB3D613D63E}"/>
+    <hyperlink ref="A236" r:id="rId116" display="https://ecos.fws.gov/ecp/species/6542" xr:uid="{DADE2C4D-0227-984F-8F70-BD2D0C8B169C}"/>
+    <hyperlink ref="A237" r:id="rId117" display="https://ecos.fws.gov/ecp/species/3812" xr:uid="{FB209C52-F21A-AF44-B559-18D122CB78CD}"/>
+    <hyperlink ref="A238" r:id="rId118" display="https://ecos.fws.gov/ecp/species/8915" xr:uid="{6F877B72-DF29-1A41-B332-3074BCDFC9C8}"/>
+    <hyperlink ref="A239" r:id="rId119" display="https://ecos.fws.gov/ecp/species/4532" xr:uid="{E1987221-660D-1644-B48C-5F791F1C3C2E}"/>
+    <hyperlink ref="A240" r:id="rId120" display="https://ecos.fws.gov/ecp/species/9827" xr:uid="{2D51B487-5D39-0843-A37E-FA40ADD408D6}"/>
+    <hyperlink ref="A241" r:id="rId121" display="https://ecos.fws.gov/ecp/species/5071" xr:uid="{F7C139B6-F278-C44D-848D-63F91B5C85C6}"/>
+    <hyperlink ref="A242" r:id="rId122" display="https://ecos.fws.gov/ecp/species/9832" xr:uid="{E2277873-671A-1845-809D-3BC28AC6C186}"/>
+    <hyperlink ref="A243" r:id="rId123" display="https://ecos.fws.gov/ecp/species/6252" xr:uid="{75ADEA4D-4E00-EF4A-9E26-8022DC586754}"/>
+    <hyperlink ref="A244" r:id="rId124" display="https://ecos.fws.gov/ecp/species/6815" xr:uid="{4AFC468D-A9FE-BB4D-9851-9BB54453E642}"/>
+    <hyperlink ref="A245" r:id="rId125" display="https://ecos.fws.gov/ecp/species/9837" xr:uid="{4AF342DA-11D9-AC49-9B84-50CEC76DFA53}"/>
+    <hyperlink ref="A333" r:id="rId126" display="https://ecos.fws.gov/ecp/species/5908" xr:uid="{A66DDBD4-E9EF-E344-8EF4-AA102BC5CE50}"/>
+    <hyperlink ref="A334" r:id="rId127" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=K007" xr:uid="{154407DE-4A70-FD48-95B6-5F264B73D503}"/>
+    <hyperlink ref="A335" r:id="rId128" display="https://ecos.fws.gov/ecp/species/3150" xr:uid="{12B65F36-DF9E-F94C-B891-007649A291E7}"/>
+    <hyperlink ref="A336" r:id="rId129" display="https://ecos.fws.gov/ecp/species/7901" xr:uid="{BA3DE6B8-A1DF-5E42-92E0-9F7345A48D75}"/>
+    <hyperlink ref="A337" r:id="rId130" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=K04R" xr:uid="{919A27E2-9F84-8B42-80E1-A566D0ADA50D}"/>
+    <hyperlink ref="A12" r:id="rId131" display="https://ecos.fws.gov/ecp/species/3966" xr:uid="{6A4C802F-39BC-C043-AFBF-47D182426F3D}"/>
+    <hyperlink ref="A65" r:id="rId132" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=E0AR" xr:uid="{B94DF11E-3BB4-EE4D-AC8E-1EFEB90B39B8}"/>
+    <hyperlink ref="A73" r:id="rId133" display="https://ecos.fws.gov/ecp/species/5634" xr:uid="{2FEE5F92-AD02-B044-92AD-59BF79229CA6}"/>
+    <hyperlink ref="A78" r:id="rId134" display="https://ecos.fws.gov/ecp/species/5162" xr:uid="{5BA51E07-DF2C-E843-BB27-39EA050713BE}"/>
+    <hyperlink ref="A79" r:id="rId135" display="https://ecos.fws.gov/ecp/species/5883" xr:uid="{0BBC2D63-CDA5-4746-9D42-EEC73B64A316}"/>
+    <hyperlink ref="A88" r:id="rId136" display="https://ecos.fws.gov/ecp/species/5605" xr:uid="{4367DD89-7045-5A4C-AA50-910A6F89BF12}"/>
+    <hyperlink ref="A96" r:id="rId137" display="https://ecos.fws.gov/ecp/species/9851" xr:uid="{04157E71-1250-8C4C-8569-D3E20F37EFFF}"/>
+    <hyperlink ref="A99" r:id="rId138" display="https://ecos.fws.gov/ecp/species/5601" xr:uid="{19B03DAE-CDDD-3242-80DE-40A817488237}"/>
+    <hyperlink ref="A100" r:id="rId139" display="https://ecos.fws.gov/ecp/species/3117" xr:uid="{D9B8D077-FE01-6F41-AEDA-0A7DCB1D1C02}"/>
+    <hyperlink ref="A101" r:id="rId140" display="https://ecos.fws.gov/ecp/species/4984" xr:uid="{97D9F208-52A1-A248-83BC-B4C7049505B2}"/>
+    <hyperlink ref="A103" r:id="rId141" display="https://ecos.fws.gov/ecp/species/9852" xr:uid="{41A119D1-1FCF-AD4E-9980-710F9917976F}"/>
+    <hyperlink ref="A104" r:id="rId142" display="https://ecos.fws.gov/ecp/species/1396" xr:uid="{F5035606-4266-8148-8759-8A95CDC8847E}"/>
+    <hyperlink ref="A105" r:id="rId143" display="https://ecos.fws.gov/ecp/species/300" xr:uid="{55D943C2-8BFC-8246-8893-82EC311A6A8E}"/>
+    <hyperlink ref="A106" r:id="rId144" display="https://ecos.fws.gov/ecp/species/9854" xr:uid="{7F0F2FE9-E9BA-DE4B-A68E-265EB2FD7919}"/>
+    <hyperlink ref="A107" r:id="rId145" display="https://ecos.fws.gov/ecp/species/8219" xr:uid="{CF79CE6E-FEFF-D64D-AD3C-4C5B4B1641D7}"/>
+    <hyperlink ref="A124" r:id="rId146" display="https://ecos.fws.gov/ecp/species/9171" xr:uid="{A6B499D7-22C0-A140-BFF9-0167DB934640}"/>
+    <hyperlink ref="A125" r:id="rId147" display="https://ecos.fws.gov/ecp/species/5045" xr:uid="{9F3E29E7-3F1C-2D44-BBA0-B415A9F35381}"/>
+    <hyperlink ref="A129" r:id="rId148" display="https://ecos.fws.gov/ecp/species/627" xr:uid="{05BB08E2-B70B-984A-9ABA-BB9AB2506A0D}"/>
+    <hyperlink ref="A157" r:id="rId149" display="https://ecos.fws.gov/ecp/species/8217" xr:uid="{42376615-CFC2-B94F-BD90-CB313B2D1484}"/>
+    <hyperlink ref="A166" r:id="rId150" display="https://ecos.fws.gov/ecp/species/9298" xr:uid="{8E89C400-051D-754D-AD85-B8B1FCB944EC}"/>
+    <hyperlink ref="A168" r:id="rId151" display="https://ecos.fws.gov/ecp/species/6899" xr:uid="{3CD8C228-179F-9542-8F92-ACDCC2E59EB7}"/>
+    <hyperlink ref="A188" r:id="rId152" display="https://ecos.fws.gov/ecp/species/9855" xr:uid="{560CB0AA-5D97-7F44-B5C8-9C3F5EA610AD}"/>
+    <hyperlink ref="A189" r:id="rId153" display="https://ecos.fws.gov/ecp/species/3931" xr:uid="{2293F100-7AA3-5C47-9F93-7A17CCD29160}"/>
+    <hyperlink ref="A190" r:id="rId154" display="https://ecos.fws.gov/ecp/species/2994" xr:uid="{C5671D86-B2E5-B344-8F39-1E5B5ABF921F}"/>
+    <hyperlink ref="A191" r:id="rId155" display="https://ecos.fws.gov/ecp/species/528" xr:uid="{C0C0588C-4EA7-3B4B-86E5-C88838FCC5A7}"/>
+    <hyperlink ref="A192" r:id="rId156" display="https://ecos.fws.gov/ecp/species/3120" xr:uid="{FF835422-50C8-1840-A5B0-D081B0D9E598}"/>
+    <hyperlink ref="A193" r:id="rId157" display="https://ecos.fws.gov/ecp/species/9861" xr:uid="{A6ECB29D-F146-C34C-BA9B-EC9AA79A5EAF}"/>
+    <hyperlink ref="A194" r:id="rId158" display="https://ecos.fws.gov/ecp/species/2800" xr:uid="{1AF230A5-D505-A44F-B357-B894599D81AF}"/>
+    <hyperlink ref="A195" r:id="rId159" display="https://ecos.fws.gov/ecp/species/2576" xr:uid="{613C4046-2DF5-5244-88F4-0F47A736B92F}"/>
+    <hyperlink ref="A214" r:id="rId160" display="https://ecos.fws.gov/ecp/species/9863" xr:uid="{7B1C05F6-BE4C-1443-A55D-D32DA5532DD0}"/>
+    <hyperlink ref="A215" r:id="rId161" display="https://ecos.fws.gov/ecp/species/6211" xr:uid="{E325B52F-5C96-F34C-9476-35EB20E37748}"/>
+    <hyperlink ref="A216" r:id="rId162" display="https://ecos.fws.gov/ecp/species/9864" xr:uid="{9CD96110-BC8C-924E-B6D3-EF8CA0A61FAD}"/>
+    <hyperlink ref="A217" r:id="rId163" display="https://ecos.fws.gov/ecp/species/5431" xr:uid="{16D4A496-E1C7-7141-BDD7-276F725021B3}"/>
+    <hyperlink ref="A218" r:id="rId164" display="https://ecos.fws.gov/ecp/species/1773" xr:uid="{2CB73C16-3985-FC43-AAFD-9FAEE4DF5FAB}"/>
+    <hyperlink ref="A219" r:id="rId165" display="https://ecos.fws.gov/ecp/species/9866" xr:uid="{F914A8AF-884A-4C4E-B108-CCFEA654F885}"/>
+    <hyperlink ref="A306" r:id="rId166" display="https://ecos.fws.gov/ecp/species/3416" xr:uid="{08F039F4-252C-634C-BAF4-2B3456409F68}"/>
+    <hyperlink ref="A312" r:id="rId167" display="https://ecos.fws.gov/ecp/species/7544" xr:uid="{99EE4CF0-37B7-B747-A65B-B1FE615ABC3C}"/>
+    <hyperlink ref="A327" r:id="rId168" display="https://ecos.fws.gov/ecp/species/9011" xr:uid="{FCD9C05F-292A-1B4B-AD9E-522E77F8F511}"/>
+    <hyperlink ref="A341" r:id="rId169" display="https://ecos.fws.gov/ecp/species/9868" xr:uid="{F92A75AD-F5B8-4E42-9C87-4EFCB7AC248A}"/>
+    <hyperlink ref="A346" r:id="rId170" display="https://ecos.fws.gov/ecp/species/4398" xr:uid="{688A5CC8-471D-8D4F-B2C7-A5F48CE80690}"/>
+    <hyperlink ref="A4" r:id="rId171" display="https://ecos.fws.gov/ecp/species/9918" xr:uid="{724C8741-2014-0447-B126-860B34D0CD4A}"/>
+    <hyperlink ref="A10" r:id="rId172" display="https://ecos.fws.gov/ecp/species/2364" xr:uid="{B3955CAA-1DC9-7345-B8BB-F60AA23DE765}"/>
+    <hyperlink ref="A16" r:id="rId173" display="https://ecos.fws.gov/ecp/species/5310" xr:uid="{A3F068D6-0D9F-534D-A11E-DAA612C3C742}"/>
+    <hyperlink ref="A21" r:id="rId174" display="https://ecos.fws.gov/ecp/species/7798" xr:uid="{D93E9E4F-BBEB-6E4F-B627-B82EFAD20987}"/>
+    <hyperlink ref="A24" r:id="rId175" display="https://ecos.fws.gov/ecp/species/1300" xr:uid="{96AEE1F4-A18E-2341-B553-7FD082C12021}"/>
+    <hyperlink ref="A25" r:id="rId176" display="https://ecos.fws.gov/ecp/species/6679" xr:uid="{8AB70AC6-7481-6F4F-9EE4-2442283B23F6}"/>
+    <hyperlink ref="A26" r:id="rId177" display="https://ecos.fws.gov/ecp/species/7577" xr:uid="{BE789AC0-ADC4-FC45-9A0A-D2611684E51E}"/>
+    <hyperlink ref="A27" r:id="rId178" display="https://ecos.fws.gov/ecp/species/4807" xr:uid="{30119158-FE03-2649-B590-19D332FD0366}"/>
+    <hyperlink ref="A31" r:id="rId179" display="https://ecos.fws.gov/ecp/species/8125" xr:uid="{47D09E27-3439-CF4E-8EA5-3D7FCC0ED34C}"/>
+    <hyperlink ref="A32" r:id="rId180" display="https://ecos.fws.gov/ecp/species/5023" xr:uid="{C04191E6-C8C4-1642-9476-315C3B6E1406}"/>
+    <hyperlink ref="A33" r:id="rId181" display="https://ecos.fws.gov/ecp/species/1807" xr:uid="{1EBDEC32-9875-444A-A6EB-7881400C19A8}"/>
+    <hyperlink ref="A40" r:id="rId182" display="https://ecos.fws.gov/ecp/species/2285" xr:uid="{EB089F99-EB84-E54C-878F-94E15251CDEF}"/>
+    <hyperlink ref="A41" r:id="rId183" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=Q3P5" xr:uid="{085784BB-41F9-4E42-AC37-2AE37811F7ED}"/>
+    <hyperlink ref="A68" r:id="rId184" display="https://ecos.fws.gov/ecp/species/8963" xr:uid="{4E9A384E-3163-554E-9555-6A3C9EE328D2}"/>
+    <hyperlink ref="A72" r:id="rId185" display="https://ecos.fws.gov/ecp/species/8619" xr:uid="{FA916CD7-E9ED-2541-936D-5F891F6E94C6}"/>
+    <hyperlink ref="A47" r:id="rId186" display="https://ecos.fws.gov/ecp/species/9627" xr:uid="{06BADA9A-0F87-814D-81E1-2AF6E641F8E4}"/>
+    <hyperlink ref="A87" r:id="rId187" display="https://ecos.fws.gov/ecp/species/8736" xr:uid="{961A49D4-4271-D54C-A7E3-EF7724CB70A6}"/>
+    <hyperlink ref="A92" r:id="rId188" display="https://ecos.fws.gov/ecp/species/2375" xr:uid="{BEECF353-AE88-7947-AB0C-0C77A17D71E5}"/>
+    <hyperlink ref="A94" r:id="rId189" display="https://ecos.fws.gov/ecp/species/9927" xr:uid="{0F949A64-0A3C-D540-9FD9-EF8EAED13F68}"/>
+    <hyperlink ref="A95" r:id="rId190" display="https://ecos.fws.gov/ecp/species/9929" xr:uid="{890A6171-C275-AC47-AEC8-EB04860B1DE3}"/>
+    <hyperlink ref="A97" r:id="rId191" display="https://ecos.fws.gov/ecp/species/2841" xr:uid="{557863FF-6902-1049-89D2-CE513BF2E5A4}"/>
+    <hyperlink ref="A98" r:id="rId192" display="https://ecos.fws.gov/ecp/species/5825" xr:uid="{641A797C-6175-6F45-9CDA-01C14FDCCFCC}"/>
+    <hyperlink ref="A130" r:id="rId193" display="https://ecos.fws.gov/ecp/species/572" xr:uid="{D672B3F0-29D4-0C48-8327-D0ADF4AFC538}"/>
+    <hyperlink ref="A134" r:id="rId194" display="https://ecos.fws.gov/ecp/species/8382" xr:uid="{5728097E-CC3A-4F4A-9C68-5D0967385602}"/>
+    <hyperlink ref="A142" r:id="rId195" display="https://ecos.fws.gov/ecp/species/9933" xr:uid="{4D799BB5-0AC6-7746-8FDC-FACE634842CB}"/>
+    <hyperlink ref="A148" r:id="rId196" display="https://ecos.fws.gov/ecp/species/3833" xr:uid="{570A4D50-B04C-364F-A754-EC5C1FB7F83E}"/>
+    <hyperlink ref="A156" r:id="rId197" display="https://ecos.fws.gov/ecp/species/2378" xr:uid="{BC916449-17EF-DB41-ABC8-329B8F308A53}"/>
+    <hyperlink ref="A158" r:id="rId198" display="https://ecos.fws.gov/ecp/species/7683" xr:uid="{EF8AA05B-1D2F-AA4E-A33E-5536D0965255}"/>
+    <hyperlink ref="A167" r:id="rId199" display="https://ecos.fws.gov/ecp/species/279" xr:uid="{A5133E10-E45E-BA42-9BAE-8D3E3E17A48B}"/>
+    <hyperlink ref="A170" r:id="rId200" display="https://ecos.fws.gov/ecp/species/879" xr:uid="{52D06944-1626-3C43-BAFC-BEC4831AA5DB}"/>
+    <hyperlink ref="A176" r:id="rId201" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=Q2UP" xr:uid="{FDC6F224-EBF2-054F-AD01-BBFEFD85F731}"/>
+    <hyperlink ref="A182" r:id="rId202" display="https://ecos.fws.gov/ecp/species/3325" xr:uid="{5E2D827F-E163-2A44-8A32-562FA0DF5E23}"/>
+    <hyperlink ref="A196" r:id="rId203" display="https://ecos.fws.gov/ecp/species/9937" xr:uid="{57BE5B8A-2933-CF46-B7E8-C6269AD67EB8}"/>
+    <hyperlink ref="A211" r:id="rId204" display="https://ecos.fws.gov/ecp/species/6441" xr:uid="{4B66B831-54A4-C84D-97D3-746E534A1DA0}"/>
+    <hyperlink ref="A212" r:id="rId205" display="https://ecos.fws.gov/ecp/species/1348" xr:uid="{C94B322B-07EC-8044-AB12-7215C57DFFD0}"/>
+    <hyperlink ref="A213" r:id="rId206" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=Q3F2" xr:uid="{BAD8198E-81E6-4A4D-8466-3CDAE0203BE5}"/>
+    <hyperlink ref="A220" r:id="rId207" display="https://ecos.fws.gov/ecp/species/599" xr:uid="{29C4D3A7-9631-9C46-BC35-5E2B52F190C7}"/>
+    <hyperlink ref="A223" r:id="rId208" display="https://ecos.fws.gov/ecp/species/1748" xr:uid="{B3C2191A-0069-624E-8D91-880CE56E1E6D}"/>
+    <hyperlink ref="A311" r:id="rId209" display="https://ecos.fws.gov/ecp/species/8397" xr:uid="{EBCD1C11-392F-234B-AA3D-D64983180592}"/>
+    <hyperlink ref="A313" r:id="rId210" display="https://ecos.fws.gov/ecp/species/883" xr:uid="{A649374D-E3C9-214A-BCB8-F8CC458D100D}"/>
+    <hyperlink ref="A314" r:id="rId211" display="https://ecos.fws.gov/ecp/species/6796" xr:uid="{13F55EB7-C340-8745-89A7-02B6DA3CADFA}"/>
+    <hyperlink ref="A317" r:id="rId212" display="https://ecos.fws.gov/ecp/species/5588" xr:uid="{D6509748-8754-734A-8E23-315B55C63B2B}"/>
+    <hyperlink ref="A318" r:id="rId213" display="https://ecos.fws.gov/ecp/species/2227" xr:uid="{70627C4D-4065-7542-B7AF-A55FF597F299}"/>
+    <hyperlink ref="A328" r:id="rId214" display="https://ecos.fws.gov/ecp/species/3157" xr:uid="{8046201C-7F62-CD41-89CB-270425083D64}"/>
+    <hyperlink ref="A330" r:id="rId215" display="https://ecos.fws.gov/ecp/species/2856" xr:uid="{E7DE1317-C80C-6C44-9A49-F6F8F346EDA5}"/>
+    <hyperlink ref="A344" r:id="rId216" display="https://ecos.fws.gov/ecp/species/9029" xr:uid="{5C6A3194-DD79-3445-841B-FDC7A54EDB20}"/>
+    <hyperlink ref="A360" r:id="rId217" display="https://ecos.fws.gov/ecp/species/1848" xr:uid="{D7815388-0B25-DF4F-B284-4869D133A980}"/>
+    <hyperlink ref="A2" r:id="rId218" display="https://ecos.fws.gov/ecp/species/9914" xr:uid="{A7A8C81D-056E-9B4B-8E64-EAE14931388A}"/>
+    <hyperlink ref="A20" r:id="rId219" display="https://ecos.fws.gov/ecp/species/9141" xr:uid="{250B8AB4-08B0-EC4B-A5B2-2EEFCF37120F}"/>
+    <hyperlink ref="A28" r:id="rId220" display="https://ecos.fws.gov/ecp/species/8601" xr:uid="{080E1ED8-C529-464D-AFD1-B04E3AA126FE}"/>
+    <hyperlink ref="A29" r:id="rId221" display="https://ecos.fws.gov/ecp/species/9005" xr:uid="{2CC35D3C-B66D-9A42-912F-6B32580E6422}"/>
+    <hyperlink ref="A30" r:id="rId222" display="https://ecos.fws.gov/ecp/species/8270" xr:uid="{E21D9869-7AB0-5A41-9B30-04202DF00EE2}"/>
+    <hyperlink ref="A42" r:id="rId223" display="https://ecos.fws.gov/ecp/species/7022" xr:uid="{EC4ABD3A-5CD9-9249-9AB4-FE6E936A3F4E}"/>
+    <hyperlink ref="A44" r:id="rId224" display="https://ecos.fws.gov/ecp/species/10403" xr:uid="{E1F7BC20-0ECC-0D4F-9C30-31FF11E7C55C}"/>
+    <hyperlink ref="A66" r:id="rId225" display="https://ecos.fws.gov/ecp/species/8134" xr:uid="{E8B8C5A0-5B0F-9C44-B6A3-51A16B942EA1}"/>
+    <hyperlink ref="A67" r:id="rId226" display="https://ecos.fws.gov/ecp/species/9982" xr:uid="{2B1635C7-02F3-1344-B67F-5A9340CD6BDC}"/>
+    <hyperlink ref="A71" r:id="rId227" display="https://ecos.fws.gov/ecp/species/9053" xr:uid="{60700EB9-3856-B34E-877C-64D025ABDA49}"/>
+    <hyperlink ref="A81" r:id="rId228" display="https://ecos.fws.gov/ecp/species/9743" xr:uid="{A05FC1A8-19BB-ED4E-AA32-50F3B9D608F7}"/>
+    <hyperlink ref="A108" r:id="rId229" display="https://ecos.fws.gov/ecp/species/3285" xr:uid="{0237321C-939C-DC48-9D5B-498BE5D56A8D}"/>
+    <hyperlink ref="A111" r:id="rId230" display="https://ecos.fws.gov/ecp/species/9209" xr:uid="{4833C1BB-1050-0D4E-A21F-725D719C97F8}"/>
+    <hyperlink ref="A112" r:id="rId231" display="https://ecos.fws.gov/ecp/species/9208" xr:uid="{8129E995-3DB7-3F42-B602-EFB261DF1067}"/>
+    <hyperlink ref="A113" r:id="rId232" display="https://ecos.fws.gov/ecp/species/9779" xr:uid="{5BF7124A-71C1-B345-835F-8B9E48B7DDC3}"/>
+    <hyperlink ref="A114" r:id="rId233" display="https://ecos.fws.gov/ecp/species/9781" xr:uid="{E0E7C544-F570-0348-82AD-7D52CE929A08}"/>
+    <hyperlink ref="A140" r:id="rId234" display="https://ecos.fws.gov/ecp/species/5618" xr:uid="{873F2B97-CACF-B84E-B745-E87604F1B592}"/>
+    <hyperlink ref="A146" r:id="rId235" display="https://ecos.fws.gov/ecp/species/8768" xr:uid="{DB10DE9D-21BA-474A-905F-6003EC0088F9}"/>
+    <hyperlink ref="A155" r:id="rId236" display="https://ecos.fws.gov/ecp/species/5640" xr:uid="{DB718CDE-F7B5-B740-9C37-F7FA50FB58C6}"/>
+    <hyperlink ref="A173" r:id="rId237" display="https://ecos.fws.gov/ecp/species/8852" xr:uid="{BA298C64-9585-FF4C-B230-7677A828FFA6}"/>
+    <hyperlink ref="A174" r:id="rId238" display="https://ecos.fws.gov/ecp/species/8602" xr:uid="{E747DA66-A794-AC40-9460-47C328CA02E2}"/>
+    <hyperlink ref="A175" r:id="rId239" display="https://ecos.fws.gov/ecp/species/4379" xr:uid="{9ABB73AE-4990-AC43-B625-F7F7577E0A39}"/>
+    <hyperlink ref="A184" r:id="rId240" display="https://ecos.fws.gov/ecp/species/6613" xr:uid="{4BCD9FF3-13F7-EF44-8585-CD3860F30541}"/>
+    <hyperlink ref="A201" r:id="rId241" display="https://ecos.fws.gov/ecp/species/3057" xr:uid="{0FE754B7-4B8D-0046-A5CF-A932B60510AD}"/>
+    <hyperlink ref="A210" r:id="rId242" display="https://ecos.fws.gov/ecp/species/7863" xr:uid="{5F6B341E-4C77-D74C-BDA8-00E3B7C0913D}"/>
+    <hyperlink ref="A247" r:id="rId243" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=I0J3" xr:uid="{90801182-17AC-FE41-BCC7-988F7E617A17}"/>
+    <hyperlink ref="A248" r:id="rId244" display="https://ecos.fws.gov/ecp/species/6127" xr:uid="{3D8F9A2A-C5E6-8C40-9A3E-A3B4E4B73488}"/>
+    <hyperlink ref="A249" r:id="rId245" display="https://ecos.fws.gov/ecp/species/2819" xr:uid="{EEEB47C7-85F6-E540-B47B-6921201DB40B}"/>
+    <hyperlink ref="A250" r:id="rId246" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=I0JH" xr:uid="{5810F599-D671-5849-A592-9913575BD4CC}"/>
+    <hyperlink ref="A251" r:id="rId247" display="https://ecos.fws.gov/ecp/species/6531" xr:uid="{6A27090F-899D-F24B-9052-3324BA73EB7B}"/>
+    <hyperlink ref="A252" r:id="rId248" display="https://ecos.fws.gov/ecp/species/1411" xr:uid="{4E00BB03-A026-8C4F-8AC1-13F5A5434DCD}"/>
+    <hyperlink ref="A253" r:id="rId249" display="https://ecos.fws.gov/ecp/species/3401" xr:uid="{42ABB0C5-55E3-5A43-BA11-9255629917A1}"/>
+    <hyperlink ref="A254" r:id="rId250" display="https://ecos.fws.gov/ecp/species/6128" xr:uid="{5D956EE9-D9E5-1D49-88D5-4EA884B01BD9}"/>
+    <hyperlink ref="A255" r:id="rId251" display="https://ecos.fws.gov/ecp/species/6075" xr:uid="{E66E3689-F6B9-084C-BD2D-423923BEE121}"/>
+    <hyperlink ref="A256" r:id="rId252" display="https://ecos.fws.gov/ecp/species/3142" xr:uid="{1FB67122-101D-724A-B599-33EC6127AB47}"/>
+    <hyperlink ref="A257" r:id="rId253" display="https://ecos.fws.gov/ecp/species/8016" xr:uid="{4AA23102-D4D0-B744-B7B7-9C01C235B996}"/>
+    <hyperlink ref="A258" r:id="rId254" display="https://ecos.fws.gov/ecp/species/8223" xr:uid="{26374774-4461-454F-A511-0A216584F004}"/>
+    <hyperlink ref="A259" r:id="rId255" display="https://ecos.fws.gov/ecp/species/1791" xr:uid="{432BE856-44B7-6540-832F-E8E962B272ED}"/>
+    <hyperlink ref="A260" r:id="rId256" display="https://ecos.fws.gov/ecp/species/7174" xr:uid="{97EA6E83-6060-8E45-A4EB-CBAFB0D1FDA4}"/>
+    <hyperlink ref="A261" r:id="rId257" display="https://ecos.fws.gov/ecp/species/8537" xr:uid="{E0A10225-0CEE-034F-AC4A-13628805ADF7}"/>
+    <hyperlink ref="A262" r:id="rId258" display="https://ecos.fws.gov/ecp/species/5059" xr:uid="{65C791CD-5C49-734F-B334-616228F2935B}"/>
+    <hyperlink ref="A263" r:id="rId259" display="https://ecos.fws.gov/ecp/species/7025" xr:uid="{6E3A68D4-5C44-0044-BC46-A70348A69CCC}"/>
+    <hyperlink ref="A264" r:id="rId260" display="https://ecos.fws.gov/ecp/species/5654" xr:uid="{B1A49F6A-2F10-F84B-B451-A4546A238067}"/>
+    <hyperlink ref="A307" r:id="rId261" display="https://ecos.fws.gov/ecp/species/9869" xr:uid="{22E1137B-5F2A-8E4E-B3F5-CC3566EB25A1}"/>
+    <hyperlink ref="A308" r:id="rId262" display="https://ecos.fws.gov/ecp/species/218" xr:uid="{5A1DDA99-40E0-F342-AF7F-2CA489CDEA8B}"/>
+    <hyperlink ref="A319" r:id="rId263" display="https://ecos.fws.gov/ecp/species/7553" xr:uid="{5C24E9C7-0708-074F-8B69-86188E79D7D5}"/>
+    <hyperlink ref="A324" r:id="rId264" display="https://ecos.fws.gov/ecp/species/8145" xr:uid="{29F1D7EF-F1B0-5446-A0E5-F44C70387EAA}"/>
+    <hyperlink ref="A325" r:id="rId265" display="https://ecos.fws.gov/ecp/species/2813" xr:uid="{1D55CFD7-98A4-8C4C-A051-ADAE1DF78334}"/>
+    <hyperlink ref="A338" r:id="rId266" display="https://ecos.fws.gov/ecp/species/9924" xr:uid="{F9F8FDEC-2856-DF47-8ADF-95AE578B0DB8}"/>
+    <hyperlink ref="A19" r:id="rId267" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=A0J3" xr:uid="{9FCD13C7-987A-D949-B48A-6D79074E5C25}"/>
+    <hyperlink ref="A77" r:id="rId268" display="https://ecos.fws.gov/ecp/species/7401" xr:uid="{0F1BEB22-6A53-F044-AFB9-50F72D858F56}"/>
+    <hyperlink ref="A85" r:id="rId269" display="https://ecos.fws.gov/ecp/species/2985" xr:uid="{75786265-65B3-BB49-8FA6-1A7399ACAB86}"/>
+    <hyperlink ref="A136" r:id="rId270" display="https://ecos.fws.gov/ecp/species/5123" xr:uid="{FD5FED9D-31FC-684C-B13D-7D769F82ABBB}"/>
+    <hyperlink ref="A179" r:id="rId271" display="https://ecos.fws.gov/ecp/species/3651" xr:uid="{433D049B-B6D4-5842-83EA-B5D564DFB021}"/>
+    <hyperlink ref="A185" r:id="rId272" display="https://ecos.fws.gov/ecp/species/9051" xr:uid="{F3A8D873-9F74-8A4D-8EC2-1FE366D9B4E0}"/>
+    <hyperlink ref="A199" r:id="rId273" display="https://ecos.fws.gov/ecp/species/8791" xr:uid="{DA852D23-8E67-384A-9BD7-2732CBC6F45B}"/>
+    <hyperlink ref="A326" r:id="rId274" display="https://ecos.fws.gov/ecp/species/2984" xr:uid="{EC605DE9-D94C-034D-BE0F-12435E45F89B}"/>
+    <hyperlink ref="A339" r:id="rId275" display="https://ecos.fws.gov/ecp/species/5126" xr:uid="{AD56C8A9-43E9-DE45-9FE4-695D1AAB2D76}"/>
+    <hyperlink ref="A362" r:id="rId276" display="https://ecos.fws.gov/ecp/species/4252" xr:uid="{2AB82B5D-CBA6-444F-A35C-5C7B3A732A32}"/>
+    <hyperlink ref="A181" r:id="rId277" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=S02V" xr:uid="{B2D70AAF-A561-8B46-ADBC-3512B3A130B4}"/>
+    <hyperlink ref="A226" r:id="rId278" display="https://ecos.fws.gov/ecp/species/8100" xr:uid="{E8057E05-FB62-FA47-8784-979385D8981C}"/>
+    <hyperlink ref="A3" r:id="rId279" display="https://ecos.fws.gov/ecp/species/1833" xr:uid="{63A9D92A-E637-FC41-A5C4-C48CFBE5341C}"/>
+    <hyperlink ref="A22" r:id="rId280" display="https://ecos.fws.gov/ecp/species/8793" xr:uid="{C06B57C4-A1F3-574F-9B5D-E7ECF80F6014}"/>
+    <hyperlink ref="A64" r:id="rId281" display="https://ecos.fws.gov/ecp/species/3525" xr:uid="{58D710FD-1276-1B4F-9FFC-555FFC4FC942}"/>
+    <hyperlink ref="A70" r:id="rId282" display="https://ecos.fws.gov/ecp/species/4979" xr:uid="{090965A1-13D4-5942-A72D-95754AECA1A4}"/>
+    <hyperlink ref="A82" r:id="rId283" display="https://ecos.fws.gov/ecp/species/9903" xr:uid="{1760FEB8-C0A4-4544-B969-827C32C37499}"/>
+    <hyperlink ref="A84" r:id="rId284" display="https://ecos.fws.gov/ecp/species/6768" xr:uid="{15B7D83E-9237-D24F-8C24-899F7A4405A9}"/>
+    <hyperlink ref="A89" r:id="rId285" display="https://ecos.fws.gov/ecp/species/47" xr:uid="{4C8B457F-ECC3-8649-B838-9AFF1812ACAE}"/>
+    <hyperlink ref="A93" r:id="rId286" display="https://ecos.fws.gov/ecp/species/6056" xr:uid="{87815E7C-C47F-734B-B3CB-371329D3D8FE}"/>
+    <hyperlink ref="A109" r:id="rId287" display="https://ecos.fws.gov/ecp/species/4480" xr:uid="{0A9A51F2-0791-C242-B88F-2CFCF4F7F700}"/>
+    <hyperlink ref="A110" r:id="rId288" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=C050" xr:uid="{C3CD780A-497A-9D43-A4E5-91CC8169047F}"/>
+    <hyperlink ref="A131" r:id="rId289" display="https://ecos.fws.gov/ecp/species/6997" xr:uid="{9FD2F6F8-D3E1-D548-B92A-2DE68426B6A3}"/>
+    <hyperlink ref="A132" r:id="rId290" display="https://ecos.fws.gov/ecp/species/6994" xr:uid="{C9FD3986-569A-AC4C-8192-2A2201FDDEF1}"/>
+    <hyperlink ref="A133" r:id="rId291" display="https://ecos.fws.gov/ecp/species/3085" xr:uid="{4E41431E-D574-A243-AB6C-95BDC760D6AB}"/>
+    <hyperlink ref="A147" r:id="rId292" display="https://ecos.fws.gov/ecp/species/3248" xr:uid="{8B63A8A7-6BA6-D445-B7D0-CF7E8DA3C724}"/>
+    <hyperlink ref="A152" r:id="rId293" display="https://ecos.fws.gov/ecp/species/9044" xr:uid="{6027797E-5D96-BA4B-B225-8BF7990F2BF0}"/>
+    <hyperlink ref="A178" r:id="rId294" display="https://ecos.fws.gov/ecp/species/4658" xr:uid="{998C2B89-AC49-8D42-B490-0188A82A89E0}"/>
+    <hyperlink ref="A225" r:id="rId295" display="https://ecos.fws.gov/ecp/species/4978" xr:uid="{DE885E6C-C66F-E549-ACC0-8839B33A5818}"/>
+    <hyperlink ref="A266" r:id="rId296" display="https://ecos.fws.gov/ecp/species/9957" xr:uid="{89C6D7CC-174C-D04E-9F56-2AE08A646C10}"/>
+    <hyperlink ref="A316" r:id="rId297" display="https://ecos.fws.gov/ecp/species/9087" xr:uid="{5E752F79-2715-8943-814B-53E97A27F8DE}"/>
+    <hyperlink ref="A329" r:id="rId298" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=C07C" xr:uid="{B794AB29-7FDC-C44D-921D-0492B07800AA}"/>
+    <hyperlink ref="A340" r:id="rId299" display="https://ecos.fws.gov/ecp/species/1497" xr:uid="{9748C32F-9C8D-2145-BB52-2B28630A320F}"/>
+    <hyperlink ref="A75" r:id="rId300" display="https://ecos.fws.gov/ecp/species/294" xr:uid="{4997B699-FEFB-2243-AF81-C1838D2B55CD}"/>
+    <hyperlink ref="A76" r:id="rId301" display="https://ecos.fws.gov/ecp/species/8598" xr:uid="{F88EA5DA-6E14-B94A-8ED1-49EDA381ACC2}"/>
+    <hyperlink ref="A83" r:id="rId302" display="https://ecos.fws.gov/ecp/species/8642" xr:uid="{1833321D-A53C-264B-83A0-A5D48C450F84}"/>
+    <hyperlink ref="A90" r:id="rId303" display="https://ecos.fws.gov/ecp/species/9896" xr:uid="{D06B3CB6-BF50-8048-9351-C7BDC1F36794}"/>
+    <hyperlink ref="A145" r:id="rId304" display="https://ecos.fws.gov/ecp/species/8641" xr:uid="{4B9F62CF-D1B9-DA49-AAD2-9E6A4F025A79}"/>
+    <hyperlink ref="A169" r:id="rId305" display="https://ecos.fws.gov/ecp/species/9911" xr:uid="{7ABF6ED7-BDE7-0247-B9C7-20C92D8F63C2}"/>
+    <hyperlink ref="A183" r:id="rId306" display="https://ecos.fws.gov/ecp/species/4369" xr:uid="{5F1EBB6A-AA1F-5145-BA40-FBD8E49A96ED}"/>
+    <hyperlink ref="A209" r:id="rId307" display="https://ecos.fws.gov/ecp0/profile/speciesProfile?spcode=G0EB" xr:uid="{773F7FBA-0F90-4645-B8C6-3C012182D921}"/>
+    <hyperlink ref="A221" r:id="rId308" display="https://ecos.fws.gov/ecp/species/7006" xr:uid="{50B3DD9B-EAEB-3349-84FB-0AF848F3F20F}"/>
+    <hyperlink ref="A227" r:id="rId309" display="https://ecos.fws.gov/ecp/species/6216" xr:uid="{9730A146-ED06-2945-A97C-E5D0F28699EA}"/>
+    <hyperlink ref="A269" r:id="rId310" display="https://ecos.fws.gov/ecp/species/4987" xr:uid="{45CCE743-EB0E-EA4D-8F86-3FDAE65F5E28}"/>
+    <hyperlink ref="A270" r:id="rId311" display="https://ecos.fws.gov/ecp/species/8978" xr:uid="{5A4CCFF5-7CC1-054F-A702-FEB18266A8B4}"/>
+    <hyperlink ref="A271" r:id="rId312" display="https://ecos.fws.gov/ecp/species/8979" xr:uid="{33263263-43E6-7F42-8BFA-4ED660757361}"/>
+    <hyperlink ref="A272" r:id="rId313" display="https://ecos.fws.gov/ecp/species/9913" xr:uid="{A501B99B-BE81-F741-85EC-E7253F89E413}"/>
+    <hyperlink ref="A273" r:id="rId314" display="https://ecos.fws.gov/ecp/species/8980" xr:uid="{7BA54CAF-17CC-4C4F-97D0-2D292EDCF695}"/>
+    <hyperlink ref="A274" r:id="rId315" display="https://ecos.fws.gov/ecp/species/4830" xr:uid="{4E5E779F-CF5D-F240-A459-C8504FE32B7D}"/>
+    <hyperlink ref="A275" r:id="rId316" display="https://ecos.fws.gov/ecp/species/8981" xr:uid="{A88140F5-20E6-1B49-A5CD-40BFD2AA9ACC}"/>
+    <hyperlink ref="A276" r:id="rId317" display="https://ecos.fws.gov/ecp/species/7545" xr:uid="{86E13FCB-E819-534E-AC7A-904CB81463F2}"/>
+    <hyperlink ref="A277" r:id="rId318" display="https://ecos.fws.gov/ecp/species/1399" xr:uid="{FFB68022-6D9D-4241-B712-CE30B0F26D02}"/>
+    <hyperlink ref="A278" r:id="rId319" display="https://ecos.fws.gov/ecp/species/8982" xr:uid="{B9010237-DB8E-1F4C-BB10-986E55F870B8}"/>
+    <hyperlink ref="A280" r:id="rId320" display="https://ecos.fws.gov/ecp/species/8985" xr:uid="{91F0E7F3-3706-DF45-9A43-EBAB7360A45B}"/>
+    <hyperlink ref="A281" r:id="rId321" display="https://ecos.fws.gov/ecp/species/1380" xr:uid="{CCBE3125-7253-FE4E-9710-731F17350D8E}"/>
+    <hyperlink ref="A283" r:id="rId322" display="https://ecos.fws.gov/ecp/species/8987" xr:uid="{8DAB7C63-A47B-184C-AA21-D8C1546BDBBF}"/>
+    <hyperlink ref="A284" r:id="rId323" display="https://ecos.fws.gov/ecp/species/8989" xr:uid="{15C90215-F1E3-2D4C-8EF6-2250991B556B}"/>
+    <hyperlink ref="A285" r:id="rId324" display="https://ecos.fws.gov/ecp/species/4778" xr:uid="{A59CDD50-28BF-FC4E-8296-9ABF8E70B868}"/>
+    <hyperlink ref="A286" r:id="rId325" display="https://ecos.fws.gov/ecp/species/5868" xr:uid="{548937D9-B0E1-E948-A300-3187CB9380CE}"/>
+    <hyperlink ref="A290" r:id="rId326" display="https://ecos.fws.gov/ecp/species/8994" xr:uid="{31B494FE-14D6-B542-8562-B692EEE42EEC}"/>
+    <hyperlink ref="A293" r:id="rId327" display="https://ecos.fws.gov/ecp/species/8996" xr:uid="{03C32A2F-A893-5E49-B35D-3B060D992EE9}"/>
+    <hyperlink ref="A297" r:id="rId328" display="https://ecos.fws.gov/ecp/species/9000" xr:uid="{7AB68529-EA6D-B54B-B2B9-9002B1897920}"/>
+    <hyperlink ref="A320" r:id="rId329" display="https://ecos.fws.gov/ecp/species/1015" xr:uid="{3DA46EB9-EFA1-A346-A3A0-BB03A6121C1B}"/>
+    <hyperlink ref="A321" r:id="rId330" display="https://ecos.fws.gov/ecp/species/7840" xr:uid="{4B10B1E8-9209-8D4C-BAD2-CC9CCE215434}"/>
+    <hyperlink ref="A322" r:id="rId331" display="https://ecos.fws.gov/ecp/species/4377" xr:uid="{735B4EDF-A337-AD40-94B5-0EC887206D30}"/>
+    <hyperlink ref="A345" r:id="rId332" display="https://ecos.fws.gov/ecp/species/8849" xr:uid="{A22843EF-9822-8640-B572-BF13BEA9CEF0}"/>
+    <hyperlink ref="A349" r:id="rId333" display="https://ecos.fws.gov/ecp/species/6645" xr:uid="{AB3ED14A-8398-8340-8DDF-4CB07D95CC2B}"/>
+    <hyperlink ref="A350" r:id="rId334" display="https://ecos.fws.gov/ecp/species/303" xr:uid="{09E6B8E2-F3DA-A249-8845-6241DDE97B65}"/>
+    <hyperlink ref="A351" r:id="rId335" display="https://ecos.fws.gov/ecp/species/7837" xr:uid="{323C5521-385F-3749-BD80-9C796736583E}"/>
+    <hyperlink ref="A352" r:id="rId336" display="https://ecos.fws.gov/ecp/species/2556" xr:uid="{E65B2E6A-16DB-9049-A799-DE3605A1D06F}"/>
+    <hyperlink ref="A353" r:id="rId337" display="https://ecos.fws.gov/ecp/species/4521" xr:uid="{A27A40CA-50B3-9445-A36B-D2170709F07C}"/>
+    <hyperlink ref="A354" r:id="rId338" display="https://ecos.fws.gov/ecp/species/6906" xr:uid="{D435C3D7-C2FD-094D-8B5A-6F242AD663F0}"/>
+    <hyperlink ref="A357" r:id="rId339" display="https://ecos.fws.gov/ecp/species/8761" xr:uid="{A4D83D16-B766-1648-AABF-2621C8BF7767}"/>
+    <hyperlink ref="A358" r:id="rId340" display="https://ecos.fws.gov/ecp/species/8850" xr:uid="{931D2621-747D-1249-9F78-6506CAA2814A}"/>
+    <hyperlink ref="A359" r:id="rId341" display="https://ecos.fws.gov/ecp/species/8896" xr:uid="{44846242-77B0-2244-B039-0F1F776F32F1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>